<commit_message>
Added Wheelwriter 1500 to keyboard_matrix.xls.  [Thanks to Chris Coley.] Added wheelwriter_1500_user_manual.pdf.         [ " ]
</commit_message>
<xml_diff>
--- a/docs/wheelwriter/keyboard_matrix.xlsx
+++ b/docs/wheelwriter/keyboard_matrix.xlsx
@@ -1,29 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave\Desktop\IBM 1620 Jr\Console Typewriter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cygwin\home\Dave\github\Cadetwriter\docs\wheelwriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CCA8D8-DA62-465C-89AC-794CA037CE8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484B42B2-5B3F-46E2-8181-FA62E884EEC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{5E82A069-CE49-40B7-9E46-07FE8FC3DAB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5E82A069-CE49-40B7-9E46-07FE8FC3DAB8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Wheelwriter" sheetId="2" r:id="rId1"/>
-    <sheet name="WW Keyboard" sheetId="5" r:id="rId2"/>
-    <sheet name="IBM 1620" sheetId="3" r:id="rId3"/>
-    <sheet name="IBM 1620 Keyboard" sheetId="9" r:id="rId4"/>
-    <sheet name="ASCII" sheetId="4" r:id="rId5"/>
-    <sheet name="ASCII Keyboard" sheetId="10" r:id="rId6"/>
+    <sheet name="Wheelwriter 1000" sheetId="2" r:id="rId1"/>
+    <sheet name="WW 1000 Keyboard" sheetId="5" r:id="rId2"/>
+    <sheet name="Wheelwriter 1500" sheetId="11" r:id="rId3"/>
+    <sheet name="WW 1500 Keyboard" sheetId="12" r:id="rId4"/>
+    <sheet name="IBM 1620" sheetId="3" r:id="rId5"/>
+    <sheet name="IBM 1620 Keyboard" sheetId="9" r:id="rId6"/>
+    <sheet name="ASCII" sheetId="4" r:id="rId7"/>
+    <sheet name="ASCII Keyboard" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">ASCII!$A$1:$Q$13</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'IBM 1620'!$A$1:$Q$13</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Wheelwriter!$A$1:$Q$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">ASCII!$A$1:$Q$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'IBM 1620'!$A$1:$Q$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Wheelwriter 1000'!$A$1:$Q$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Wheelwriter 1500'!$A$1:$Q$13</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="253">
-  <si>
-    <t>Wheelwriter Typewriter</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="288">
   <si>
     <t>KYBD-8
 J14-8</t>
@@ -5058,13 +5058,345 @@
     <t xml:space="preserve">(76)
 ESC
 </t>
+  </si>
+  <si>
+    <t>Wheelwriter 1500 Typewriter</t>
+  </si>
+  <si>
+    <t>J1-4</t>
+  </si>
+  <si>
+    <t>J1-14</t>
+  </si>
+  <si>
+    <t>J1-5</t>
+  </si>
+  <si>
+    <t>J1-2</t>
+  </si>
+  <si>
+    <t>J1-15</t>
+  </si>
+  <si>
+    <t>J1-6</t>
+  </si>
+  <si>
+    <t>J1-7</t>
+  </si>
+  <si>
+    <t>J1-8</t>
+  </si>
+  <si>
+    <t>J1-9</t>
+  </si>
+  <si>
+    <t>J1-10</t>
+  </si>
+  <si>
+    <t>J1-11</t>
+  </si>
+  <si>
+    <t>J1-12</t>
+  </si>
+  <si>
+    <t>J1-13</t>
+  </si>
+  <si>
+    <t>J1-3</t>
+  </si>
+  <si>
+    <t>KYBD-8
+J2-8</t>
+  </si>
+  <si>
+    <t>KYBD-9
+J2-9</t>
+  </si>
+  <si>
+    <t>KYBD-10
+J2-10</t>
+  </si>
+  <si>
+    <t>KYBD-11
+J2-11</t>
+  </si>
+  <si>
+    <t>KYBD-12
+J2-12</t>
+  </si>
+  <si>
+    <t>KYBD-13
+J2-13</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(76)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mar Rel</t>
+    </r>
+  </si>
+  <si>
+    <t>KYBD-14
+J2-14</t>
+  </si>
+  <si>
+    <t>KYBD-15
+J2-15</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">key #, unshifted (key #), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shifted (key # + 78, shift: 0x0101/0x0102)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>code (key # + 156, shift: 0x0501)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unavailable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(17)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dir</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(19)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Phrs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(20)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RePrt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(21)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mark</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(67)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Label</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(68)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Envip</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(70)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Forms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(78)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Page Eject</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Key available on all Wheelwriters</t>
+  </si>
+  <si>
+    <t>Key available on Wheelwriter 1500</t>
+  </si>
+  <si>
+    <t>Wheelwriter 1000 Typewriter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5151,8 +5483,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5165,8 +5504,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -5390,11 +5735,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5495,6 +5877,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5579,6 +5985,61 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>80182</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBE83A79-188B-44A1-9383-4B44B746E688}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10058400" cy="2556682"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>50390</xdr:rowOff>
     </xdr:to>
@@ -5622,7 +6083,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -5977,9 +6438,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5991,13 +6452,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>0</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="D2" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -6015,514 +6476,523 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="J3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="8" t="s">
+      <c r="N3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33"/>
       <c r="B5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="L5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="M5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="N5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="P5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="Q5" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>39</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>40</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
       <c r="O6" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N7" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q7" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N8" s="15"/>
       <c r="O8" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P8" s="15"/>
       <c r="Q8" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M9" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N9" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O9" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P9" s="29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q9" s="25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K10" s="23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N10" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O10" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P10" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q10" s="16"/>
     </row>
     <row r="11" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M11" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N11" s="15"/>
       <c r="O11" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P11" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q11" s="25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K12" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M12" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P12" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q12" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
       <c r="O13" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P13" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q13" s="30" t="s">
-        <v>169</v>
-      </c>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="38" t="s">
+        <v>285</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B16:D16"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
@@ -6536,9 +7006,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -6549,6 +7017,598 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB534B26-C33B-4205-9104-627328F4B974}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="17" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="D2" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
+      <c r="B5" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q6" s="26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="L7" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="O7" s="15"/>
+      <c r="P7" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q7" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="M8" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="N8" s="15"/>
+      <c r="O8" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="O9" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="P9" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q9" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="L10" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="N10" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="O10" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="P10" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q10" s="16"/>
+    </row>
+    <row r="11" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>279</v>
+      </c>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="M11" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="N11" s="15"/>
+      <c r="O11" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q11" s="25" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="O12" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="P12" s="36" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q12" s="25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="P13" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q13" s="37" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="38" t="s">
+        <v>285</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="40"/>
+    </row>
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="41" t="s">
+        <v>286</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B18:D18"/>
+  </mergeCells>
+  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9EE706-5CC0-4610-8D75-4AA82A7EF88B}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4109A74B-AC4B-4E91-81EA-85E169682ACC}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6567,13 +7627,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="D2" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -6591,249 +7651,249 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="J3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="8" t="s">
+      <c r="N3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33"/>
       <c r="B5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="L5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="M5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="N5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="P5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="Q5" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
       <c r="O6" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N7" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q7" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="15"/>
@@ -6843,75 +7903,75 @@
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M8" s="27"/>
       <c r="N8" s="15"/>
       <c r="O8" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P8" s="15"/>
       <c r="Q8" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="27"/>
       <c r="F9" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M9" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N9" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O9" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P9" s="15"/>
       <c r="Q9" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="15"/>
@@ -6921,141 +7981,141 @@
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
       <c r="K10" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N10" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O10" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="P10" s="15"/>
       <c r="Q10" s="16"/>
     </row>
     <row r="11" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M11" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N11" s="15"/>
       <c r="O11" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="P11" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Q11" s="25" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="27"/>
       <c r="F12" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K12" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M12" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="P12" s="15"/>
       <c r="Q12" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
       <c r="O13" s="24" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P13" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q13" s="19"/>
     </row>
@@ -7069,16 +8129,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91ED9149-F662-4131-826E-0EFAA9070053}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -7088,14 +8146,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{140E5FB2-DF83-4FAE-B108-99043006927A}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7107,13 +8165,13 @@
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="D2" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -7131,251 +8189,251 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="J3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="8" t="s">
+      <c r="N3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33"/>
       <c r="B5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="L5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="M5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="N5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="P5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="Q5" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
       <c r="O6" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q6" s="26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="23" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K7" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N7" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O7" s="15"/>
       <c r="P7" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q7" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="15"/>
@@ -7385,229 +8443,229 @@
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N8" s="15"/>
       <c r="O8" s="23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P8" s="15"/>
       <c r="Q8" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K9" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M9" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N9" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O9" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P9" s="15"/>
       <c r="Q9" s="25" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="15"/>
       <c r="F10" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K10" s="23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L10" s="23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M10" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N10" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O10" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P10" s="15"/>
       <c r="Q10" s="16"/>
     </row>
     <row r="11" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M11" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N11" s="15"/>
       <c r="O11" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P11" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Q11" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="27"/>
       <c r="F12" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K12" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M12" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O12" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P12" s="15"/>
       <c r="Q12" s="25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" s="18"/>
       <c r="G13" s="24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M13" s="18"/>
       <c r="N13" s="18"/>
       <c r="O13" s="24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P13" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q13" s="19"/>
     </row>
@@ -7621,7 +8679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608D8068-0F3A-4DB4-BDE0-37DA55020E59}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>

<commit_message>
Added print sample for each machine.
</commit_message>
<xml_diff>
--- a/docs/wheelwriter/keyboard_matrix.xlsx
+++ b/docs/wheelwriter/keyboard_matrix.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cygwin\home\Dave\github\Cadetwriter\docs\wheelwriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484B42B2-5B3F-46E2-8181-FA62E884EEC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C879B65-6F46-4D52-B058-30B0B49FC6F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5E82A069-CE49-40B7-9E46-07FE8FC3DAB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Wheelwriter 1000" sheetId="2" r:id="rId1"/>
     <sheet name="WW 1000 Keyboard" sheetId="5" r:id="rId2"/>
-    <sheet name="Wheelwriter 1500" sheetId="11" r:id="rId3"/>
-    <sheet name="WW 1500 Keyboard" sheetId="12" r:id="rId4"/>
-    <sheet name="IBM 1620" sheetId="3" r:id="rId5"/>
-    <sheet name="IBM 1620 Keyboard" sheetId="9" r:id="rId6"/>
+    <sheet name="Wheelwriter 1500" sheetId="13" r:id="rId3"/>
+    <sheet name="WW 1500 Keyboard" sheetId="14" r:id="rId4"/>
+    <sheet name="IBM 1620 Jr." sheetId="3" r:id="rId5"/>
+    <sheet name="IBM 1620 Jr. Keyboard" sheetId="9" r:id="rId6"/>
     <sheet name="ASCII" sheetId="4" r:id="rId7"/>
     <sheet name="ASCII Keyboard" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="6">ASCII!$A$1:$Q$13</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'IBM 1620'!$A$1:$Q$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'IBM 1620 Jr.'!$A$1:$Q$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Wheelwriter 1000'!$A$1:$Q$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Wheelwriter 1500'!$A$1:$Q$13</definedName>
   </definedNames>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="292">
   <si>
     <t>KYBD-8
 J14-8</t>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>teensy pin</t>
-  </si>
-  <si>
-    <t>IBM 1620 Console Typewriter</t>
   </si>
   <si>
     <r>
@@ -5060,7 +5057,81 @@
 </t>
   </si>
   <si>
+    <t>IBM 1620 Jr. Console Typewriter</t>
+  </si>
+  <si>
     <t>Wheelwriter 1500 Typewriter</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">key #, unshifted (key #), </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shifted (key # + 78, shift: 0x0101/0x0102)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>code (key # + 156, shift: 0x0501)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unavailable</t>
+    </r>
   </si>
   <si>
     <t>J1-4</t>
@@ -5117,19 +5188,104 @@
 J2-10</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">(17)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dir</t>
+    </r>
+  </si>
+  <si>
     <t>KYBD-11
 J2-11</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">(67)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Label</t>
+    </r>
+  </si>
+  <si>
     <t>KYBD-12
 J2-12</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">(19)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Phrs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(68)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Envip</t>
+    </r>
+  </si>
+  <si>
     <t>KYBD-13
 J2-13</t>
   </si>
   <si>
     <r>
+      <t xml:space="preserve">(20)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RePrt</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">(76)
 </t>
     </r>
@@ -5150,212 +5306,56 @@
 J2-14</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">(21)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mark</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(70)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Forms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
     <t>KYBD-15
 J2-15</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">key #, unshifted (key #), </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>shifted (key # + 78, shift: 0x0101/0x0102)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>code (key # + 156, shift: 0x0501)</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="4"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>unavailable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(17)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Dir</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(19)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Phrs</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(20)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RePrt</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(21)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mark</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(67)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Label</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(68)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Envip</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(70)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Forms</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">(78)
 </t>
     </r>
@@ -5390,13 +5390,25 @@
   </si>
   <si>
     <t>Wheelwriter 1000 Typewriter</t>
+  </si>
+  <si>
+    <t>Wheelwriter 1000 Keyboard</t>
+  </si>
+  <si>
+    <t>Wheelwriter 1500 Keyboard</t>
+  </si>
+  <si>
+    <t>IBM 1620 Jr. Keyboard</t>
+  </si>
+  <si>
+    <t>ASCII Keyboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5479,13 +5491,6 @@
       <i/>
       <sz val="11"/>
       <color theme="4"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5776,7 +5781,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5807,9 +5812,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -5868,6 +5870,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5877,16 +5883,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5924,13 +5931,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>112984</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5970,6 +5977,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419093</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C953850-5A6D-477D-A847-B3E4CA4670CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3048000"/>
+          <a:ext cx="10172693" cy="847725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5979,13 +6036,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>80182</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5993,7 +6050,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBE83A79-188B-44A1-9383-4B44B746E688}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16B99A5B-7B1E-4F56-9CA2-1B0742445186}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6025,6 +6082,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419093</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DA8F5FA-839E-4BA0-BF0C-E181F8FE4317}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2857500"/>
+          <a:ext cx="10172693" cy="847725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6034,13 +6141,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>50390</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6080,6 +6187,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>320718</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76F73E12-0961-4DA0-BC50-49DB238ED332}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3047999"/>
+          <a:ext cx="10074318" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6089,13 +6246,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>112192</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6127,6 +6284,56 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="10058400" cy="2779192"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>439402</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25D00B38-9984-47AF-977A-FA0848A16286}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050" y="3067050"/>
+          <a:ext cx="10173952" cy="752475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6438,9 +6645,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6451,28 +6660,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="35" t="s">
         <v>287</v>
       </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
+      <c r="D2" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -6522,8 +6734,8 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>76</v>
+      <c r="A4" s="33" t="s">
+        <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
@@ -6572,9 +6784,9 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>40</v>
@@ -6630,39 +6842,39 @@
         <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q6" s="26" t="s">
-        <v>162</v>
+      <c r="F6" s="13"/>
+      <c r="G6" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q6" s="25" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -6673,133 +6885,133 @@
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="L7" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="N7" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="O7" s="15"/>
-      <c r="P7" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q7" s="25" t="s">
-        <v>163</v>
+      <c r="E7" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="O7" s="14"/>
+      <c r="P7" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="M8" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="N8" s="15"/>
-      <c r="O8" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="25" t="s">
-        <v>164</v>
+        <v>67</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="N8" s="14"/>
+      <c r="O8" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="24" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="K9" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="L9" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="N9" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="O9" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="P9" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q9" s="25" t="s">
-        <v>165</v>
+        <v>68</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="P9" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q9" s="24" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -6810,44 +7022,44 @@
         <v>4</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="K10" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="L10" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="N10" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="O10" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="P10" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q10" s="16"/>
+        <v>69</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="P10" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q10" s="15"/>
     </row>
     <row r="11" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -6857,39 +7069,39 @@
         <v>5</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="L11" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="M11" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="N11" s="15"/>
-      <c r="O11" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="P11" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q11" s="25" t="s">
-        <v>166</v>
+        <v>70</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="N11" s="14"/>
+      <c r="O11" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q11" s="24" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -6900,45 +7112,45 @@
         <v>6</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="L12" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="M12" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="N12" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="O12" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="P12" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q12" s="25" t="s">
-        <v>167</v>
+        <v>71</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="O12" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="P12" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q12" s="24" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6949,50 +7161,42 @@
         <v>7</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="P13" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q13" s="30" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="38" t="s">
-        <v>285</v>
-      </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="40"/>
+        <v>72</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="L13" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="P13" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q13" s="29" t="s">
+        <v>167</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
@@ -7004,12 +7208,32 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>288</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -7017,13 +7241,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB534B26-C33B-4205-9104-627328F4B974}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC43BC9B-8D7A-4B8E-A3E5-1296FC84C70F}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7034,28 +7260,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="35" t="s">
         <v>252</v>
       </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="31" t="s">
-        <v>276</v>
-      </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
+      <c r="D2" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -7105,59 +7334,59 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>76</v>
+      <c r="A4" s="33" t="s">
+        <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34" t="s">
-        <v>64</v>
+      <c r="A5" s="34"/>
+      <c r="B5" s="37" t="s">
+        <v>63</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>40</v>
@@ -7210,42 +7439,42 @@
         <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q6" s="26" t="s">
-        <v>162</v>
+      <c r="F6" s="13"/>
+      <c r="G6" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q6" s="25" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7253,136 +7482,136 @@
         <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="L7" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="N7" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="O7" s="15"/>
-      <c r="P7" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q7" s="25" t="s">
-        <v>163</v>
+      <c r="E7" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="O7" s="14"/>
+      <c r="P7" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="35" t="s">
-        <v>277</v>
-      </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="M8" s="23" t="s">
-        <v>139</v>
-      </c>
-      <c r="N8" s="15"/>
-      <c r="O8" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="25" t="s">
-        <v>164</v>
+        <v>67</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="N8" s="14"/>
+      <c r="O8" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="24" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="K9" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="L9" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="N9" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="O9" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="P9" s="35" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q9" s="25" t="s">
-        <v>165</v>
+        <v>68</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="P9" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q9" s="24" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7390,89 +7619,89 @@
         <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>278</v>
-      </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="K10" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="L10" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="N10" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="O10" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="P10" s="36" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q10" s="16"/>
+        <v>69</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="P10" s="38" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q10" s="15"/>
     </row>
     <row r="11" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>278</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="N11" s="14"/>
+      <c r="O11" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q11" s="24" t="s">
         <v>279</v>
-      </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="L11" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="M11" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="N11" s="15"/>
-      <c r="O11" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="P11" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q11" s="25" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7480,48 +7709,48 @@
         <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>280</v>
-      </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>128</v>
-      </c>
-      <c r="L12" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="M12" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="N12" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="O12" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="P12" s="36" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q12" s="25" t="s">
-        <v>167</v>
+        <v>71</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="O12" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="P12" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q12" s="24" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7529,62 +7758,63 @@
         <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="P13" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q13" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="L13" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="P13" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q13" s="39" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="40" t="s">
         <v>285</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
     </row>
     <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="43" t="s">
         <v>286</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="40"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
@@ -7592,16 +7822,36 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9EE706-5CC0-4610-8D75-4AA82A7EF88B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B88EFCA-45C9-4577-BFCB-BF965314A1F6}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -7615,7 +7865,9 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7626,28 +7878,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>62</v>
-      </c>
+      <c r="A1" s="35" t="s">
+        <v>251</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
+      <c r="D2" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -7697,8 +7952,8 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>76</v>
+      <c r="A4" s="33" t="s">
+        <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
@@ -7747,9 +8002,9 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>40</v>
@@ -7805,38 +8060,38 @@
         <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q6" s="28"/>
+      <c r="E6" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q6" s="27"/>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -7846,121 +8101,121 @@
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="L7" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="N7" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="O7" s="15"/>
-      <c r="P7" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q7" s="25" t="s">
-        <v>163</v>
+      <c r="E7" s="14"/>
+      <c r="F7" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="O7" s="14"/>
+      <c r="P7" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="M8" s="27"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="25" t="s">
-        <v>164</v>
+        <v>67</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="M8" s="26"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="24" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="K9" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="L9" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="N9" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="O9" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="25" t="s">
-        <v>213</v>
+        <v>68</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="24" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7971,32 +8226,32 @@
         <v>4</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="L10" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="N10" s="23" t="s">
-        <v>200</v>
-      </c>
-      <c r="O10" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="16"/>
+        <v>69</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="15"/>
     </row>
     <row r="11" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -8006,37 +8261,37 @@
         <v>5</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="L11" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="M11" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="N11" s="15"/>
-      <c r="O11" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="P11" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q11" s="25" t="s">
-        <v>214</v>
+        <v>70</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="N11" s="14"/>
+      <c r="O11" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q11" s="24" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8047,39 +8302,39 @@
         <v>6</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="L12" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="M12" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="N12" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="O12" s="23" t="s">
-        <v>207</v>
-      </c>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="25" t="s">
-        <v>167</v>
+        <v>71</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="O12" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="24" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8090,39 +8345,40 @@
         <v>7</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="P13" s="24" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q13" s="19"/>
+        <v>72</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="L13" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="P13" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q13" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="96" fitToWidth="0" orientation="landscape" r:id="rId1"/>
@@ -8134,12 +8390,32 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -8153,7 +8429,9 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8164,28 +8442,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>65</v>
-      </c>
+      <c r="A1" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="36"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
+      <c r="D2" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -8235,8 +8514,8 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>76</v>
+      <c r="A4" s="33" t="s">
+        <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
@@ -8285,9 +8564,9 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>40</v>
@@ -8343,39 +8622,39 @@
         <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="P6" s="22" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q6" s="26" t="s">
-        <v>250</v>
+      <c r="E6" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q6" s="25" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8386,125 +8665,125 @@
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>225</v>
-      </c>
-      <c r="L7" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="N7" s="23" t="s">
-        <v>242</v>
-      </c>
-      <c r="O7" s="15"/>
-      <c r="P7" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="Q7" s="25" t="s">
-        <v>163</v>
+      <c r="E7" s="14"/>
+      <c r="F7" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="O7" s="14"/>
+      <c r="P7" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="23" t="s">
-        <v>226</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="M8" s="23" t="s">
-        <v>239</v>
-      </c>
-      <c r="N8" s="15"/>
-      <c r="O8" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="25" t="s">
-        <v>164</v>
+        <v>67</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="N8" s="14"/>
+      <c r="O8" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="24" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="K9" s="23" t="s">
-        <v>227</v>
-      </c>
-      <c r="L9" s="23" t="s">
-        <v>234</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="N9" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="O9" s="23" t="s">
-        <v>247</v>
-      </c>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="25" t="s">
-        <v>213</v>
+        <v>68</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="24" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8515,38 +8794,38 @@
         <v>4</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>222</v>
-      </c>
-      <c r="K10" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="L10" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="N10" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="O10" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="16"/>
+        <v>69</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="15"/>
     </row>
     <row r="11" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -8556,37 +8835,37 @@
         <v>5</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="L11" s="23" t="s">
-        <v>235</v>
-      </c>
-      <c r="M11" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="N11" s="15"/>
-      <c r="O11" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="P11" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q11" s="25" t="s">
-        <v>251</v>
+        <v>70</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="N11" s="14"/>
+      <c r="O11" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q11" s="24" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8597,39 +8876,39 @@
         <v>6</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>223</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>229</v>
-      </c>
-      <c r="L12" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="M12" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="N12" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="O12" s="23" t="s">
-        <v>248</v>
-      </c>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="25" t="s">
-        <v>167</v>
+        <v>71</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="O12" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="24" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8640,39 +8919,40 @@
         <v>7</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>237</v>
-      </c>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="24" t="s">
-        <v>249</v>
-      </c>
-      <c r="P13" s="24" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q13" s="19"/>
+        <v>72</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="L13" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="P13" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q13" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="96" fitToWidth="0" orientation="landscape" r:id="rId1"/>
@@ -8684,12 +8964,32 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="31"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Updated keyboard matrix spreadsheet with Wheelwriter 1500. Added ISO/IEC escape sequence documentation. Added Paul Williamson's 3D-printable paper guide.
</commit_message>
<xml_diff>
--- a/docs/wheelwriter/keyboard_matrix.xlsx
+++ b/docs/wheelwriter/keyboard_matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cygwin\home\Dave\github\Cadetwriter\docs\wheelwriter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave\Desktop\IBM 1620 Jr\Console Typewriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C879B65-6F46-4D52-B058-30B0B49FC6F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40B3D41-7E22-4943-BB08-DF8EEA7EB179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5E82A069-CE49-40B7-9E46-07FE8FC3DAB8}"/>
   </bookViews>
@@ -21,10 +21,13 @@
     <sheet name="IBM 1620 Jr. Keyboard" sheetId="9" r:id="rId6"/>
     <sheet name="ASCII" sheetId="4" r:id="rId7"/>
     <sheet name="ASCII Keyboard" sheetId="10" r:id="rId8"/>
+    <sheet name="IBM 1620 Max" sheetId="11" r:id="rId9"/>
+    <sheet name="IBM 1620 Max Keyboard" sheetId="12" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="6">ASCII!$A$1:$Q$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'IBM 1620 Jr.'!$A$1:$Q$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">'IBM 1620 Max'!$A$1:$Q$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Wheelwriter 1000'!$A$1:$Q$13</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Wheelwriter 1500'!$A$1:$Q$13</definedName>
   </definedNames>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="335">
   <si>
     <t>KYBD-8
 J14-8</t>
@@ -1202,23 +1205,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">(16)
-&lt;load paper&gt;
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;set top of form&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">(17)
 </t>
     </r>
@@ -5057,7 +5043,558 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">(76)
+FLG
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(69)
+R-S
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(8)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;record mark&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;group mark&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(5)
+\
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(10)
+z
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Z</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(11)
+q
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Q</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(13)
+~
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>`</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(14)
+a
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(24)
+x
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(25)
+w
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>W</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(27)
+s
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>S</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(28)
+c
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(29)
+e
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(31)
+d
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(32)
+b
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(40)
+n
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(33)
+v
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>V</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(41)
+m
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(34)
+t
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(42)
+y
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(35)
+r
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(43)
+u
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>U</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(38)
+f
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(46)
+j
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(39)
+g
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>G</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(47)
+h
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H</t>
+    </r>
+  </si>
+  <si>
+    <t>(49)
+]
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(50)
+I
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(53)
+k
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>K</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(57)
+l
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(55)
+o
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>O</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(59)
+[
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(60)
+p
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P</t>
+    </r>
+  </si>
+  <si>
     <t>IBM 1620 Jr. Console Typewriter</t>
+  </si>
+  <si>
+    <t>IBM 1620 Max Console Typewriter</t>
   </si>
   <si>
     <t>Wheelwriter 1500 Typewriter</t>
@@ -5247,23 +5784,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">(68)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Envip</t>
-    </r>
-  </si>
-  <si>
     <t>KYBD-13
 J2-13</t>
   </si>
@@ -5402,13 +5922,362 @@
   </si>
   <si>
     <t>ASCII Keyboard</t>
+  </si>
+  <si>
+    <t>IBM 1620 Max Keyboard</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(22)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T Clr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Zone</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(77)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T Set</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Col L</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(29)
+e
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ExLsp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(38)
+f
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Frmat</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(46)
+j
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>J</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Jstify</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(61)
+0
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Draw</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(60)
+p
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ExPrt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(68)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Envlp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(16)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;load paper&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;set top of form&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(16)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;load paper&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5491,6 +6360,14 @@
       <i/>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5874,6 +6751,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5887,15 +6773,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6345,6 +7222,61 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>112192</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC9ABF1B-70D6-43FA-A48B-C7D185D3CDB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10058400" cy="2779192"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6660,31 +7592,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>287</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
+      <c r="A1" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -6734,7 +7666,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -6784,7 +7716,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -6855,26 +7787,26 @@
         <v>89</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
       <c r="O6" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -6897,33 +7829,33 @@
         <v>84</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>105</v>
+        <v>333</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O7" s="14"/>
       <c r="P7" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -6942,27 +7874,27 @@
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -6983,35 +7915,35 @@
         <v>85</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N9" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O9" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P9" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7032,32 +7964,32 @@
         <v>86</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N10" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O10" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P10" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q10" s="15"/>
     </row>
@@ -7079,29 +8011,29 @@
         <v>87</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7122,35 +8054,35 @@
         <v>88</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P12" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q12" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7169,27 +8101,27 @@
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P13" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q13" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -7200,6 +8132,43 @@
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678F452A-16A6-4636-A978-C09B2B13D726}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7217,12 +8186,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>288</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
+      <c r="A1" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -7260,31 +8229,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>252</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
+      <c r="A1" s="38" t="s">
+        <v>285</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="32" t="s">
-        <v>253</v>
-      </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
+      <c r="D2" s="35" t="s">
+        <v>286</v>
+      </c>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -7334,58 +8303,58 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>254</v>
+        <v>287</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>255</v>
+        <v>288</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>256</v>
+        <v>289</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>257</v>
+        <v>290</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>258</v>
+        <v>291</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>259</v>
+        <v>292</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>260</v>
+        <v>293</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>261</v>
+        <v>294</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>262</v>
+        <v>295</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>263</v>
+        <v>296</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>264</v>
+        <v>297</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>265</v>
+        <v>298</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>266</v>
+        <v>299</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>267</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
-      <c r="B5" s="37" t="s">
+      <c r="A5" s="37"/>
+      <c r="B5" s="32" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -7439,7 +8408,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>268</v>
+        <v>301</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>65</v>
@@ -7455,26 +8424,26 @@
         <v>89</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
       <c r="O6" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7482,7 +8451,7 @@
         <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>269</v>
+        <v>302</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>66</v>
@@ -7497,33 +8466,33 @@
         <v>84</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>105</v>
+        <v>333</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O7" s="14"/>
       <c r="P7" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7531,7 +8500,7 @@
         <v>73</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>270</v>
+        <v>303</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>67</v>
@@ -7541,28 +8510,28 @@
         <v>77</v>
       </c>
       <c r="F8" s="14"/>
-      <c r="G8" s="38" t="s">
-        <v>271</v>
+      <c r="G8" s="33" t="s">
+        <v>304</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7570,7 +8539,7 @@
         <v>74</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>272</v>
+        <v>305</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>68</v>
@@ -7583,35 +8552,35 @@
         <v>85</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>118</v>
+        <v>327</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N9" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O9" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="P9" s="38" t="s">
-        <v>273</v>
+        <v>331</v>
+      </c>
+      <c r="P9" s="33" t="s">
+        <v>306</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7619,7 +8588,7 @@
         <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>274</v>
+        <v>307</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>69</v>
@@ -7631,33 +8600,33 @@
       <c r="F10" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="G10" s="38" t="s">
-        <v>275</v>
+      <c r="G10" s="33" t="s">
+        <v>308</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N10" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O10" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="P10" s="38" t="s">
-        <v>276</v>
+        <v>330</v>
+      </c>
+      <c r="P10" s="33" t="s">
+        <v>332</v>
       </c>
       <c r="Q10" s="15"/>
     </row>
@@ -7666,7 +8635,7 @@
         <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>277</v>
+        <v>309</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>70</v>
@@ -7678,30 +8647,30 @@
       <c r="F11" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="38" t="s">
-        <v>278</v>
+      <c r="G11" s="33" t="s">
+        <v>310</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -7709,7 +8678,7 @@
         <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>280</v>
+        <v>312</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>71</v>
@@ -7721,36 +8690,36 @@
       <c r="F12" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="38" t="s">
-        <v>281</v>
+      <c r="G12" s="33" t="s">
+        <v>313</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>127</v>
+        <v>328</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>135</v>
+        <v>329</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="P12" s="38" t="s">
-        <v>282</v>
+        <v>151</v>
+      </c>
+      <c r="P12" s="33" t="s">
+        <v>314</v>
       </c>
       <c r="Q12" s="24" t="s">
-        <v>166</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7758,7 +8727,7 @@
         <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>283</v>
+        <v>315</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>72</v>
@@ -7769,33 +8738,33 @@
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="23" t="s">
-        <v>111</v>
+        <v>325</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P13" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q13" s="39" t="s">
-        <v>284</v>
+        <v>159</v>
+      </c>
+      <c r="Q13" s="34" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="40" t="s">
-        <v>285</v>
+        <v>317</v>
       </c>
       <c r="C16" s="41"/>
       <c r="D16" s="42"/>
@@ -7803,7 +8772,7 @@
     <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="43" t="s">
-        <v>286</v>
+        <v>318</v>
       </c>
       <c r="C18" s="41"/>
       <c r="D18" s="42"/>
@@ -7828,19 +8797,19 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>289</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
+      <c r="A1" s="38" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -7878,31 +8847,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>251</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
+      <c r="A1" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -7952,7 +8921,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -8002,7 +8971,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -8073,23 +9042,23 @@
         <v>97</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
       <c r="O6" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q6" s="27"/>
     </row>
@@ -8111,33 +9080,33 @@
         <v>104</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>168</v>
+        <v>334</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O7" s="14"/>
       <c r="P7" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8158,19 +9127,19 @@
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M8" s="26"/>
       <c r="N8" s="14"/>
       <c r="O8" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8189,33 +9158,33 @@
         <v>94</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N9" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O9" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8236,19 +9205,19 @@
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
       <c r="K10" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N10" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O10" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
@@ -8275,23 +9244,23 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8312,29 +9281,29 @@
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8353,24 +9322,24 @@
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="P13" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q13" s="18"/>
     </row>
@@ -8399,12 +9368,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>290</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
+      <c r="A1" s="38" t="s">
+        <v>322</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -8442,29 +9411,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="39"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -8514,7 +9483,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="36" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -8564,7 +9533,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -8635,26 +9604,26 @@
         <v>97</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
       <c r="O6" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8675,33 +9644,33 @@
         <v>99</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O7" s="14"/>
       <c r="P7" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8722,21 +9691,21 @@
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8757,33 +9726,33 @@
         <v>100</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N9" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O9" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8804,25 +9773,25 @@
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N10" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O10" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
@@ -8849,23 +9818,23 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -8886,29 +9855,29 @@
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8927,24 +9896,24 @@
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P13" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q13" s="18"/>
     </row>
@@ -8973,11 +9942,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>291</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
+      <c r="A1" s="38" t="s">
+        <v>323</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8994,4 +9963,543 @@
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24288E6-1965-4EA0-B3CE-F0797C610302}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="17" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="D2" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="37"/>
+      <c r="B5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q6" s="27"/>
+    </row>
+    <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="O7" s="14"/>
+      <c r="P7" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="N8" s="14"/>
+      <c r="O8" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="24" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" s="14"/>
+      <c r="I9" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="24" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="15"/>
+    </row>
+    <row r="11" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="N11" s="14"/>
+      <c r="O11" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q11" s="24" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="O12" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="L13" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="P13" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q13" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup scale="96" fitToWidth="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added ASCII printwheel character set and printwheel character ordering.
</commit_message>
<xml_diff>
--- a/docs/wheelwriter/keyboard_matrix.xlsx
+++ b/docs/wheelwriter/keyboard_matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave\Desktop\IBM 1620 Jr\Console Typewriter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cygwin\home\Dave\github\Cadetwriter\docs\wheelwriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40B3D41-7E22-4943-BB08-DF8EEA7EB179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58E4E7C-70FC-48B2-A80C-7B811FF8290E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5E82A069-CE49-40B7-9E46-07FE8FC3DAB8}"/>
+    <workbookView xWindow="435" yWindow="30" windowWidth="19875" windowHeight="10995" xr2:uid="{5E82A069-CE49-40B7-9E46-07FE8FC3DAB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Wheelwriter 1000" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="ASCII Keyboard" sheetId="10" r:id="rId8"/>
     <sheet name="IBM 1620 Max" sheetId="11" r:id="rId9"/>
     <sheet name="IBM 1620 Max Keyboard" sheetId="12" r:id="rId10"/>
+    <sheet name="Wheelwriter Printwheels" sheetId="15" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="6">ASCII!$A$1:$Q$13</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="524">
   <si>
     <t>KYBD-8
 J14-8</t>
@@ -6271,13 +6272,580 @@
       </rPr>
       <t>&lt;load paper&gt;</t>
     </r>
+  </si>
+  <si>
+    <t>Wheelwriter Printwheel Positions</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Std.</t>
+  </si>
+  <si>
+    <t>ASCII</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>noshift</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>0x09</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>0x0B</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>0x0D</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>shift</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0x0F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>0x10</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>0x11</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>0x12</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>0x13</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>0x14</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>0x15</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>0x16</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>0x17</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>0x18</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>0x19</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>0x1A</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>0x1B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>0x1C</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>0x1D</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>0x1E</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>0x1F</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>0x21</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>0x22</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>0x23</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>0x24</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>0x25</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>0x26</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>0x27</t>
+  </si>
+  <si>
+    <t>0x28</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>0x29</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>0x2A</t>
+  </si>
+  <si>
+    <t>0x2B</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>0x2C</t>
+  </si>
+  <si>
+    <t>0x2D</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>0x2E</t>
+  </si>
+  <si>
+    <t>0x2F</t>
+  </si>
+  <si>
+    <t>0x30</t>
+  </si>
+  <si>
+    <t>0x31</t>
+  </si>
+  <si>
+    <t>0x32</t>
+  </si>
+  <si>
+    <t>0x33</t>
+  </si>
+  <si>
+    <t>0x34</t>
+  </si>
+  <si>
+    <t>0x35</t>
+  </si>
+  <si>
+    <t>0x36</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>0x37</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>0x38</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>0x39</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>0x3A</t>
+  </si>
+  <si>
+    <t>¢</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>0x3B</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>0x3C</t>
+  </si>
+  <si>
+    <t>±</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>0x3D</t>
+  </si>
+  <si>
+    <t>@</t>
+  </si>
+  <si>
+    <t>0x3E</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>0x3F</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>0x40</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>0x41</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>0x42</t>
+  </si>
+  <si>
+    <t>²</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>0x43</t>
+  </si>
+  <si>
+    <t>³</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>0x44</t>
+  </si>
+  <si>
+    <t>°</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>0x45</t>
+  </si>
+  <si>
+    <t>§</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>0x46</t>
+  </si>
+  <si>
+    <t>¶</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>0x47</t>
+  </si>
+  <si>
+    <t>½</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>0x48</t>
+  </si>
+  <si>
+    <t>¼</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>0x49</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>0x4A</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>0x4B</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>0x4C</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>0x4D</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>0x4E</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>0x4F</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>0x50</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>0x51</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>0x52</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>0x53</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>0x54</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>0x55</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>0x56</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>0x57</t>
+  </si>
+  <si>
+    <t>0x58</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>0x59</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>0x5A</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>0x5B</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>0x5C</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>0x5D</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>0x5E</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>0x5F</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>0x00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6372,6 +6940,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -6393,7 +6978,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -6654,11 +7239,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -6783,6 +7377,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7172,14 +7784,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>439402</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:colOff>458452</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7209,8 +7821,58 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19050" y="3067050"/>
+          <a:off x="38100" y="4476750"/>
           <a:ext cx="10173952" cy="752475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>162214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57778</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD6C0A4A-171B-476D-9324-3C0D222E32FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3476914"/>
+          <a:ext cx="10229850" cy="848064"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8172,6 +8834,1535 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA42E1F6-175A-4BE2-8B97-2ABE974B15A6}">
+  <dimension ref="A1:E102"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>335</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="48" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49" t="s">
+        <v>337</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>338</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="46">
+        <v>0</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>523</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>340</v>
+      </c>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="46">
+        <v>1</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>342</v>
+      </c>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="46">
+        <v>2</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>343</v>
+      </c>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="46">
+        <v>3</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>344</v>
+      </c>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="46">
+        <v>4</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>345</v>
+      </c>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="46">
+        <v>5</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>346</v>
+      </c>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="46">
+        <v>6</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>347</v>
+      </c>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="46">
+        <v>7</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>348</v>
+      </c>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="46">
+        <v>8</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>350</v>
+      </c>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="46">
+        <v>9</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>349</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>352</v>
+      </c>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="46">
+        <v>10</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>351</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>354</v>
+      </c>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="46">
+        <v>11</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>353</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>356</v>
+      </c>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="46">
+        <v>12</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>355</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>358</v>
+      </c>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="46">
+        <v>13</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>357</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>361</v>
+      </c>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="46">
+        <v>14</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>360</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>363</v>
+      </c>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="46">
+        <v>15</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>365</v>
+      </c>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="46">
+        <v>16</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>364</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>367</v>
+      </c>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="46">
+        <v>17</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>366</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>369</v>
+      </c>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="46">
+        <v>18</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>368</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>371</v>
+      </c>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="46">
+        <v>19</v>
+      </c>
+      <c r="B23" s="47" t="s">
+        <v>370</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>373</v>
+      </c>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="46">
+        <v>20</v>
+      </c>
+      <c r="B24" s="47" t="s">
+        <v>372</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>375</v>
+      </c>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="46">
+        <v>21</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>374</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>377</v>
+      </c>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="46">
+        <v>22</v>
+      </c>
+      <c r="B26" s="47" t="s">
+        <v>376</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>379</v>
+      </c>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="46">
+        <v>23</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>378</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>381</v>
+      </c>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="46"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="46">
+        <v>24</v>
+      </c>
+      <c r="B29" s="47" t="s">
+        <v>380</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>383</v>
+      </c>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="46">
+        <v>25</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>382</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>385</v>
+      </c>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="46">
+        <v>26</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>384</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>387</v>
+      </c>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="46">
+        <v>27</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>386</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>389</v>
+      </c>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="46">
+        <v>28</v>
+      </c>
+      <c r="B33" s="47" t="s">
+        <v>388</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>391</v>
+      </c>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="46">
+        <v>29</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>390</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>393</v>
+      </c>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="46">
+        <v>30</v>
+      </c>
+      <c r="B35" s="47" t="s">
+        <v>392</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>395</v>
+      </c>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="46">
+        <v>31</v>
+      </c>
+      <c r="B36" s="47" t="s">
+        <v>394</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>397</v>
+      </c>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="46">
+        <v>32</v>
+      </c>
+      <c r="B37" s="47" t="s">
+        <v>396</v>
+      </c>
+      <c r="C37" s="47" t="s">
+        <v>399</v>
+      </c>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="46">
+        <v>33</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>398</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>401</v>
+      </c>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="46">
+        <v>34</v>
+      </c>
+      <c r="B39" s="47" t="s">
+        <v>400</v>
+      </c>
+      <c r="C39" s="47" t="s">
+        <v>403</v>
+      </c>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="46">
+        <v>35</v>
+      </c>
+      <c r="B40" s="47" t="s">
+        <v>402</v>
+      </c>
+      <c r="C40" s="47" t="s">
+        <v>405</v>
+      </c>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="46">
+        <v>36</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>404</v>
+      </c>
+      <c r="C41" s="47" t="s">
+        <v>407</v>
+      </c>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="46">
+        <v>37</v>
+      </c>
+      <c r="B42" s="47" t="s">
+        <v>406</v>
+      </c>
+      <c r="C42" s="47" t="s">
+        <v>409</v>
+      </c>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="46">
+        <v>38</v>
+      </c>
+      <c r="B43" s="47" t="s">
+        <v>408</v>
+      </c>
+      <c r="C43" s="47" t="s">
+        <v>356</v>
+      </c>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="46">
+        <v>39</v>
+      </c>
+      <c r="B44" s="47" t="s">
+        <v>410</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>412</v>
+      </c>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="46">
+        <v>40</v>
+      </c>
+      <c r="B45" s="47" t="s">
+        <v>411</v>
+      </c>
+      <c r="C45" s="47" t="s">
+        <v>414</v>
+      </c>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="46">
+        <v>41</v>
+      </c>
+      <c r="B46" s="47" t="s">
+        <v>413</v>
+      </c>
+      <c r="C46" s="47">
+        <v>9</v>
+      </c>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="46">
+        <v>42</v>
+      </c>
+      <c r="B47" s="47" t="s">
+        <v>415</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>417</v>
+      </c>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="46">
+        <v>43</v>
+      </c>
+      <c r="B48" s="47" t="s">
+        <v>416</v>
+      </c>
+      <c r="C48" s="47">
+        <v>3</v>
+      </c>
+      <c r="D48" s="47"/>
+      <c r="E48" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="46">
+        <v>44</v>
+      </c>
+      <c r="B49" s="47" t="s">
+        <v>418</v>
+      </c>
+      <c r="C49" s="47" t="s">
+        <v>420</v>
+      </c>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="46">
+        <v>45</v>
+      </c>
+      <c r="B50" s="47" t="s">
+        <v>419</v>
+      </c>
+      <c r="C50" s="47">
+        <v>1</v>
+      </c>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="46">
+        <v>46</v>
+      </c>
+      <c r="B51" s="47" t="s">
+        <v>421</v>
+      </c>
+      <c r="C51" s="47">
+        <v>2</v>
+      </c>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="46">
+        <v>47</v>
+      </c>
+      <c r="B52" s="47" t="s">
+        <v>422</v>
+      </c>
+      <c r="C52" s="47">
+        <v>0</v>
+      </c>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="46"/>
+      <c r="B53" s="47"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="46">
+        <v>48</v>
+      </c>
+      <c r="B54" s="47" t="s">
+        <v>423</v>
+      </c>
+      <c r="C54" s="47">
+        <v>5</v>
+      </c>
+      <c r="D54" s="47"/>
+      <c r="E54" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="46">
+        <v>49</v>
+      </c>
+      <c r="B55" s="47" t="s">
+        <v>424</v>
+      </c>
+      <c r="C55" s="47">
+        <v>4</v>
+      </c>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="46">
+        <v>50</v>
+      </c>
+      <c r="B56" s="47" t="s">
+        <v>425</v>
+      </c>
+      <c r="C56" s="47">
+        <v>6</v>
+      </c>
+      <c r="D56" s="47"/>
+      <c r="E56" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="46">
+        <v>51</v>
+      </c>
+      <c r="B57" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="C57" s="47">
+        <v>8</v>
+      </c>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="46">
+        <v>52</v>
+      </c>
+      <c r="B58" s="47" t="s">
+        <v>427</v>
+      </c>
+      <c r="C58" s="47">
+        <v>7</v>
+      </c>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="46">
+        <v>53</v>
+      </c>
+      <c r="B59" s="47" t="s">
+        <v>428</v>
+      </c>
+      <c r="C59" s="47" t="s">
+        <v>430</v>
+      </c>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="46">
+        <v>54</v>
+      </c>
+      <c r="B60" s="47" t="s">
+        <v>429</v>
+      </c>
+      <c r="C60" s="47" t="s">
+        <v>432</v>
+      </c>
+      <c r="D60" s="47"/>
+      <c r="E60" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="46">
+        <v>55</v>
+      </c>
+      <c r="B61" s="47" t="s">
+        <v>431</v>
+      </c>
+      <c r="C61" s="47" t="s">
+        <v>434</v>
+      </c>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="46">
+        <v>56</v>
+      </c>
+      <c r="B62" s="47" t="s">
+        <v>433</v>
+      </c>
+      <c r="C62" s="47" t="s">
+        <v>436</v>
+      </c>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="46">
+        <v>57</v>
+      </c>
+      <c r="B63" s="47" t="s">
+        <v>435</v>
+      </c>
+      <c r="C63" s="47" t="s">
+        <v>438</v>
+      </c>
+      <c r="D63" s="47" t="s">
+        <v>439</v>
+      </c>
+      <c r="E63" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="46">
+        <v>58</v>
+      </c>
+      <c r="B64" s="47" t="s">
+        <v>437</v>
+      </c>
+      <c r="C64" s="47" t="s">
+        <v>441</v>
+      </c>
+      <c r="D64" s="47"/>
+      <c r="E64" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="46">
+        <v>59</v>
+      </c>
+      <c r="B65" s="47" t="s">
+        <v>440</v>
+      </c>
+      <c r="C65" s="47" t="s">
+        <v>443</v>
+      </c>
+      <c r="D65" s="47" t="s">
+        <v>444</v>
+      </c>
+      <c r="E65" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="46">
+        <v>60</v>
+      </c>
+      <c r="B66" s="47" t="s">
+        <v>442</v>
+      </c>
+      <c r="C66" s="47" t="s">
+        <v>446</v>
+      </c>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="46">
+        <v>61</v>
+      </c>
+      <c r="B67" s="47" t="s">
+        <v>445</v>
+      </c>
+      <c r="C67" s="47" t="s">
+        <v>448</v>
+      </c>
+      <c r="D67" s="47"/>
+      <c r="E67" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="46">
+        <v>62</v>
+      </c>
+      <c r="B68" s="47" t="s">
+        <v>447</v>
+      </c>
+      <c r="C68" s="47" t="s">
+        <v>450</v>
+      </c>
+      <c r="D68" s="47"/>
+      <c r="E68" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="46">
+        <v>63</v>
+      </c>
+      <c r="B69" s="47" t="s">
+        <v>449</v>
+      </c>
+      <c r="C69" s="47" t="s">
+        <v>452</v>
+      </c>
+      <c r="D69" s="47"/>
+      <c r="E69" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="46">
+        <v>64</v>
+      </c>
+      <c r="B70" s="47" t="s">
+        <v>451</v>
+      </c>
+      <c r="C70" s="47" t="s">
+        <v>454</v>
+      </c>
+      <c r="D70" s="47"/>
+      <c r="E70" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="46">
+        <v>65</v>
+      </c>
+      <c r="B71" s="47" t="s">
+        <v>453</v>
+      </c>
+      <c r="C71" s="47" t="s">
+        <v>456</v>
+      </c>
+      <c r="D71" s="47" t="s">
+        <v>457</v>
+      </c>
+      <c r="E71" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="46">
+        <v>66</v>
+      </c>
+      <c r="B72" s="47" t="s">
+        <v>455</v>
+      </c>
+      <c r="C72" s="47" t="s">
+        <v>459</v>
+      </c>
+      <c r="D72" s="47" t="s">
+        <v>460</v>
+      </c>
+      <c r="E72" s="47" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="46">
+        <v>67</v>
+      </c>
+      <c r="B73" s="47" t="s">
+        <v>458</v>
+      </c>
+      <c r="C73" s="47" t="s">
+        <v>463</v>
+      </c>
+      <c r="D73" s="47" t="s">
+        <v>464</v>
+      </c>
+      <c r="E73" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="46">
+        <v>68</v>
+      </c>
+      <c r="B74" s="47" t="s">
+        <v>462</v>
+      </c>
+      <c r="C74" s="47" t="s">
+        <v>466</v>
+      </c>
+      <c r="D74" s="47" t="s">
+        <v>467</v>
+      </c>
+      <c r="E74" s="47" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="46">
+        <v>69</v>
+      </c>
+      <c r="B75" s="47" t="s">
+        <v>465</v>
+      </c>
+      <c r="C75" s="47" t="s">
+        <v>469</v>
+      </c>
+      <c r="D75" s="47" t="s">
+        <v>470</v>
+      </c>
+      <c r="E75" s="47" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="46">
+        <v>70</v>
+      </c>
+      <c r="B76" s="47" t="s">
+        <v>468</v>
+      </c>
+      <c r="C76" s="47" t="s">
+        <v>472</v>
+      </c>
+      <c r="D76" s="47" t="s">
+        <v>473</v>
+      </c>
+      <c r="E76" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="46">
+        <v>71</v>
+      </c>
+      <c r="B77" s="47" t="s">
+        <v>471</v>
+      </c>
+      <c r="C77" s="47" t="s">
+        <v>475</v>
+      </c>
+      <c r="D77" s="47" t="s">
+        <v>476</v>
+      </c>
+      <c r="E77" s="47" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="46"/>
+      <c r="B78" s="47"/>
+      <c r="C78" s="47"/>
+      <c r="D78" s="47"/>
+      <c r="E78" s="47"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="46">
+        <v>72</v>
+      </c>
+      <c r="B79" s="47" t="s">
+        <v>474</v>
+      </c>
+      <c r="C79" s="47" t="s">
+        <v>478</v>
+      </c>
+      <c r="D79" s="47"/>
+      <c r="E79" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="46">
+        <v>73</v>
+      </c>
+      <c r="B80" s="47" t="s">
+        <v>477</v>
+      </c>
+      <c r="C80" s="47" t="s">
+        <v>480</v>
+      </c>
+      <c r="D80" s="47"/>
+      <c r="E80" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="46">
+        <v>74</v>
+      </c>
+      <c r="B81" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="C81" s="47" t="s">
+        <v>482</v>
+      </c>
+      <c r="D81" s="47"/>
+      <c r="E81" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="46">
+        <v>75</v>
+      </c>
+      <c r="B82" s="47" t="s">
+        <v>481</v>
+      </c>
+      <c r="C82" s="47" t="s">
+        <v>484</v>
+      </c>
+      <c r="D82" s="47"/>
+      <c r="E82" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="46">
+        <v>76</v>
+      </c>
+      <c r="B83" s="47" t="s">
+        <v>483</v>
+      </c>
+      <c r="C83" s="47" t="s">
+        <v>486</v>
+      </c>
+      <c r="D83" s="47"/>
+      <c r="E83" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="46">
+        <v>77</v>
+      </c>
+      <c r="B84" s="47" t="s">
+        <v>485</v>
+      </c>
+      <c r="C84" s="47" t="s">
+        <v>488</v>
+      </c>
+      <c r="D84" s="47"/>
+      <c r="E84" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="46">
+        <v>78</v>
+      </c>
+      <c r="B85" s="47" t="s">
+        <v>487</v>
+      </c>
+      <c r="C85" s="47" t="s">
+        <v>490</v>
+      </c>
+      <c r="D85" s="47"/>
+      <c r="E85" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="46">
+        <v>79</v>
+      </c>
+      <c r="B86" s="47" t="s">
+        <v>489</v>
+      </c>
+      <c r="C86" s="47" t="s">
+        <v>492</v>
+      </c>
+      <c r="D86" s="47"/>
+      <c r="E86" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="46">
+        <v>80</v>
+      </c>
+      <c r="B87" s="47" t="s">
+        <v>491</v>
+      </c>
+      <c r="C87" s="47" t="s">
+        <v>494</v>
+      </c>
+      <c r="D87" s="47"/>
+      <c r="E87" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="46">
+        <v>81</v>
+      </c>
+      <c r="B88" s="47" t="s">
+        <v>493</v>
+      </c>
+      <c r="C88" s="47" t="s">
+        <v>496</v>
+      </c>
+      <c r="D88" s="47"/>
+      <c r="E88" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="46">
+        <v>82</v>
+      </c>
+      <c r="B89" s="47" t="s">
+        <v>495</v>
+      </c>
+      <c r="C89" s="47" t="s">
+        <v>498</v>
+      </c>
+      <c r="D89" s="47"/>
+      <c r="E89" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="46">
+        <v>83</v>
+      </c>
+      <c r="B90" s="47" t="s">
+        <v>497</v>
+      </c>
+      <c r="C90" s="47" t="s">
+        <v>500</v>
+      </c>
+      <c r="D90" s="47"/>
+      <c r="E90" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="46">
+        <v>84</v>
+      </c>
+      <c r="B91" s="47" t="s">
+        <v>499</v>
+      </c>
+      <c r="C91" s="47" t="s">
+        <v>502</v>
+      </c>
+      <c r="D91" s="47"/>
+      <c r="E91" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="46">
+        <v>85</v>
+      </c>
+      <c r="B92" s="47" t="s">
+        <v>501</v>
+      </c>
+      <c r="C92" s="47" t="s">
+        <v>504</v>
+      </c>
+      <c r="D92" s="47"/>
+      <c r="E92" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="46">
+        <v>86</v>
+      </c>
+      <c r="B93" s="47" t="s">
+        <v>503</v>
+      </c>
+      <c r="C93" s="47" t="s">
+        <v>407</v>
+      </c>
+      <c r="D93" s="47"/>
+      <c r="E93" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="46">
+        <v>87</v>
+      </c>
+      <c r="B94" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="C94" s="47" t="s">
+        <v>507</v>
+      </c>
+      <c r="D94" s="47"/>
+      <c r="E94" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="46">
+        <v>88</v>
+      </c>
+      <c r="B95" s="47" t="s">
+        <v>506</v>
+      </c>
+      <c r="C95" s="47" t="s">
+        <v>509</v>
+      </c>
+      <c r="D95" s="47"/>
+      <c r="E95" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="46">
+        <v>89</v>
+      </c>
+      <c r="B96" s="47" t="s">
+        <v>508</v>
+      </c>
+      <c r="C96" s="47" t="s">
+        <v>511</v>
+      </c>
+      <c r="D96" s="47"/>
+      <c r="E96" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="46">
+        <v>90</v>
+      </c>
+      <c r="B97" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="C97" s="47" t="s">
+        <v>513</v>
+      </c>
+      <c r="D97" s="47"/>
+      <c r="E97" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="46">
+        <v>91</v>
+      </c>
+      <c r="B98" s="47" t="s">
+        <v>512</v>
+      </c>
+      <c r="C98" s="47" t="s">
+        <v>515</v>
+      </c>
+      <c r="D98" s="47"/>
+      <c r="E98" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="46">
+        <v>92</v>
+      </c>
+      <c r="B99" s="47" t="s">
+        <v>514</v>
+      </c>
+      <c r="C99" s="47" t="s">
+        <v>517</v>
+      </c>
+      <c r="D99" s="47"/>
+      <c r="E99" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="46">
+        <v>93</v>
+      </c>
+      <c r="B100" s="47" t="s">
+        <v>516</v>
+      </c>
+      <c r="C100" s="47" t="s">
+        <v>519</v>
+      </c>
+      <c r="D100" s="47"/>
+      <c r="E100" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="46">
+        <v>94</v>
+      </c>
+      <c r="B101" s="47" t="s">
+        <v>518</v>
+      </c>
+      <c r="C101" s="47" t="s">
+        <v>521</v>
+      </c>
+      <c r="D101" s="47"/>
+      <c r="E101" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="46">
+        <v>95</v>
+      </c>
+      <c r="B102" s="47" t="s">
+        <v>520</v>
+      </c>
+      <c r="C102" s="47" t="s">
+        <v>522</v>
+      </c>
+      <c r="D102" s="47"/>
+      <c r="E102" s="47" t="s">
+        <v>341</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBE5D03-400C-4374-BC8E-973FA89582E6}">
   <sheetPr>

</xml_diff>

<commit_message>
Added more printwheel information.
</commit_message>
<xml_diff>
--- a/docs/wheelwriter/keyboard_matrix.xlsx
+++ b/docs/wheelwriter/keyboard_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cygwin\home\Dave\github\Cadetwriter\docs\wheelwriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E04D0F-E195-4B51-90FD-0347AB98E58A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FB23D0-86A8-44E3-B77F-BE9217146A22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="30" windowWidth="19875" windowHeight="10995" firstSheet="7" activeTab="10" xr2:uid="{5E82A069-CE49-40B7-9E46-07FE8FC3DAB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5E82A069-CE49-40B7-9E46-07FE8FC3DAB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Wheelwriter 1000" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="526">
   <si>
     <t>KYBD-8
 J14-8</t>
@@ -6839,6 +6839,12 @@
   </si>
   <si>
     <t>0x00</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Row</t>
   </si>
 </sst>
 </file>
@@ -7252,7 +7258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -7396,6 +7402,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8241,7 +8253,7 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -8836,15 +8848,18 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA42E1F6-175A-4BE2-8B97-2ABE974B15A6}">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="7" width="9.140625" style="51"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>335</v>
       </c>
@@ -8853,14 +8868,14 @@
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
       <c r="E2" s="36"/>
     </row>
-    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="49" t="s">
         <v>336</v>
       </c>
@@ -8874,8 +8889,14 @@
       <c r="E3" s="37" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="50" t="s">
+        <v>524</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="35">
         <v>0</v>
       </c>
@@ -8889,8 +8910,14 @@
       <c r="E4" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="51">
+        <v>3</v>
+      </c>
+      <c r="G4" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="35">
         <v>1</v>
       </c>
@@ -8904,8 +8931,14 @@
       <c r="E5" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="51">
+        <v>9</v>
+      </c>
+      <c r="G5" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="35">
         <v>2</v>
       </c>
@@ -8919,8 +8952,14 @@
       <c r="E6" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="51">
+        <v>8</v>
+      </c>
+      <c r="G6" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="35">
         <v>3</v>
       </c>
@@ -8934,8 +8973,14 @@
       <c r="E7" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="51">
+        <v>9</v>
+      </c>
+      <c r="G7" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="35">
         <v>4</v>
       </c>
@@ -8949,8 +8994,14 @@
       <c r="E8" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="51">
+        <v>7</v>
+      </c>
+      <c r="G8" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="35">
         <v>5</v>
       </c>
@@ -8964,8 +9015,14 @@
       <c r="E9" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="51">
+        <v>6</v>
+      </c>
+      <c r="G9" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="35">
         <v>6</v>
       </c>
@@ -8979,8 +9036,14 @@
       <c r="E10" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="51">
+        <v>7</v>
+      </c>
+      <c r="G10" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="35">
         <v>7</v>
       </c>
@@ -8994,8 +9057,14 @@
       <c r="E11" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="51">
+        <v>9</v>
+      </c>
+      <c r="G11" s="51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="35">
         <v>8</v>
       </c>
@@ -9009,8 +9078,14 @@
       <c r="E12" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="51">
+        <v>11</v>
+      </c>
+      <c r="G12" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="35">
         <v>9</v>
       </c>
@@ -9024,8 +9099,14 @@
       <c r="E13" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="51">
+        <v>8</v>
+      </c>
+      <c r="G13" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="35">
         <v>10</v>
       </c>
@@ -9039,8 +9120,14 @@
       <c r="E14" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="51">
+        <v>10</v>
+      </c>
+      <c r="G14" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="35">
         <v>11</v>
       </c>
@@ -9054,8 +9141,14 @@
       <c r="E15" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="51">
+        <v>10</v>
+      </c>
+      <c r="G15" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="35">
         <v>12</v>
       </c>
@@ -9069,8 +9162,14 @@
       <c r="E16" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="51">
+        <v>8</v>
+      </c>
+      <c r="G16" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="35">
         <v>13</v>
       </c>
@@ -9084,8 +9183,14 @@
       <c r="E17" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="51">
+        <v>12</v>
+      </c>
+      <c r="G17" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="35">
         <v>14</v>
       </c>
@@ -9099,8 +9204,14 @@
       <c r="E18" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="51">
+        <v>8</v>
+      </c>
+      <c r="G18" s="51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="35">
         <v>15</v>
       </c>
@@ -9114,8 +9225,14 @@
       <c r="E19" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="51">
+        <v>9</v>
+      </c>
+      <c r="G19" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="35">
         <v>16</v>
       </c>
@@ -9129,8 +9246,14 @@
       <c r="E20" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="51">
+        <v>8</v>
+      </c>
+      <c r="G20" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="35">
         <v>17</v>
       </c>
@@ -9144,8 +9267,14 @@
       <c r="E21" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="51">
+        <v>8</v>
+      </c>
+      <c r="G21" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="35">
         <v>18</v>
       </c>
@@ -9159,8 +9288,14 @@
       <c r="E22" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="51">
+        <v>3</v>
+      </c>
+      <c r="G22" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="35">
         <v>19</v>
       </c>
@@ -9174,8 +9309,14 @@
       <c r="E23" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="51">
+        <v>9</v>
+      </c>
+      <c r="G23" s="51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="35">
         <v>20</v>
       </c>
@@ -9189,8 +9330,14 @@
       <c r="E24" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="51">
+        <v>12</v>
+      </c>
+      <c r="G24" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="35">
         <v>21</v>
       </c>
@@ -9204,8 +9351,14 @@
       <c r="E25" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="51">
+        <v>12</v>
+      </c>
+      <c r="G25" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="35">
         <v>22</v>
       </c>
@@ -9219,8 +9372,14 @@
       <c r="E26" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="51">
+        <v>8</v>
+      </c>
+      <c r="G26" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="35">
         <v>23</v>
       </c>
@@ -9234,15 +9393,21 @@
       <c r="E27" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="51">
+        <v>11</v>
+      </c>
+      <c r="G27" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="35"/>
       <c r="B28" s="36"/>
       <c r="C28" s="36"/>
       <c r="D28" s="36"/>
       <c r="E28" s="36"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="35">
         <v>24</v>
       </c>
@@ -9256,8 +9421,14 @@
       <c r="E29" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="51">
+        <v>6</v>
+      </c>
+      <c r="G29" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="35">
         <v>25</v>
       </c>
@@ -9271,8 +9442,14 @@
       <c r="E30" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="51">
+        <v>9</v>
+      </c>
+      <c r="G30" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="35">
         <v>26</v>
       </c>
@@ -9286,8 +9463,14 @@
       <c r="E31" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="51">
+        <v>7</v>
+      </c>
+      <c r="G31" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="35">
         <v>27</v>
       </c>
@@ -9301,8 +9484,14 @@
       <c r="E32" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="51">
+        <v>8</v>
+      </c>
+      <c r="G32" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="35">
         <v>28</v>
       </c>
@@ -9316,8 +9505,14 @@
       <c r="E33" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="51">
+        <v>7</v>
+      </c>
+      <c r="G33" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="35">
         <v>29</v>
       </c>
@@ -9331,8 +9526,14 @@
       <c r="E34" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="51">
+        <v>7</v>
+      </c>
+      <c r="G34" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="35">
         <v>30</v>
       </c>
@@ -9346,8 +9547,14 @@
       <c r="E35" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="51">
+        <v>10</v>
+      </c>
+      <c r="G35" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="35">
         <v>31</v>
       </c>
@@ -9361,8 +9568,14 @@
       <c r="E36" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="51">
+        <v>3</v>
+      </c>
+      <c r="G36" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="35">
         <v>32</v>
       </c>
@@ -9376,8 +9589,14 @@
       <c r="E37" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="51">
+        <v>9</v>
+      </c>
+      <c r="G37" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="35">
         <v>33</v>
       </c>
@@ -9391,8 +9610,14 @@
       <c r="E38" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="51">
+        <v>11</v>
+      </c>
+      <c r="G38" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="35">
         <v>34</v>
       </c>
@@ -9406,8 +9631,14 @@
       <c r="E39" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="51">
+        <v>11</v>
+      </c>
+      <c r="G39" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="35">
         <v>35</v>
       </c>
@@ -9421,8 +9652,14 @@
       <c r="E40" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="51">
+        <v>9</v>
+      </c>
+      <c r="G40" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="35">
         <v>36</v>
       </c>
@@ -9436,8 +9673,14 @@
       <c r="E41" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="51">
+        <v>11</v>
+      </c>
+      <c r="G41" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="35">
         <v>37</v>
       </c>
@@ -9451,8 +9694,14 @@
       <c r="E42" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="51">
+        <v>9</v>
+      </c>
+      <c r="G42" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="35">
         <v>38</v>
       </c>
@@ -9466,8 +9715,14 @@
       <c r="E43" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="51">
+        <v>10</v>
+      </c>
+      <c r="G43" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="35">
         <v>39</v>
       </c>
@@ -9481,8 +9736,14 @@
       <c r="E44" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="51">
+        <v>12</v>
+      </c>
+      <c r="G44" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="35">
         <v>40</v>
       </c>
@@ -9496,8 +9757,14 @@
       <c r="E45" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="51">
+        <v>6</v>
+      </c>
+      <c r="G45" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="35">
         <v>41</v>
       </c>
@@ -9511,8 +9778,14 @@
       <c r="E46" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="51">
+        <v>11</v>
+      </c>
+      <c r="G46" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="35">
         <v>42</v>
       </c>
@@ -9526,8 +9799,14 @@
       <c r="E47" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="51">
+        <v>10</v>
+      </c>
+      <c r="G47" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="35">
         <v>43</v>
       </c>
@@ -9541,8 +9820,14 @@
       <c r="E48" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="51">
+        <v>7</v>
+      </c>
+      <c r="G48" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="35">
         <v>44</v>
       </c>
@@ -9556,8 +9841,14 @@
       <c r="E49" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="51">
+        <v>6</v>
+      </c>
+      <c r="G49" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="35">
         <v>45</v>
       </c>
@@ -9571,8 +9862,14 @@
       <c r="E50" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="51">
+        <v>3</v>
+      </c>
+      <c r="G50" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="35">
         <v>46</v>
       </c>
@@ -9586,8 +9883,14 @@
       <c r="E51" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="51">
+        <v>6</v>
+      </c>
+      <c r="G51" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="35">
         <v>47</v>
       </c>
@@ -9601,15 +9904,21 @@
       <c r="E52" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" s="51">
+        <v>12</v>
+      </c>
+      <c r="G52" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="35"/>
       <c r="B53" s="36"/>
       <c r="C53" s="36"/>
       <c r="D53" s="36"/>
       <c r="E53" s="36"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="35">
         <v>48</v>
       </c>
@@ -9623,8 +9932,14 @@
       <c r="E54" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="51">
+        <v>8</v>
+      </c>
+      <c r="G54" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="35">
         <v>49</v>
       </c>
@@ -9638,8 +9953,14 @@
       <c r="E55" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="51">
+        <v>8</v>
+      </c>
+      <c r="G55" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="35">
         <v>50</v>
       </c>
@@ -9653,8 +9974,14 @@
       <c r="E56" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="51">
+        <v>9</v>
+      </c>
+      <c r="G56" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="35">
         <v>51</v>
       </c>
@@ -9668,8 +9995,14 @@
       <c r="E57" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" s="51">
+        <v>10</v>
+      </c>
+      <c r="G57" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="35">
         <v>52</v>
       </c>
@@ -9683,8 +10016,14 @@
       <c r="E58" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" s="51">
+        <v>9</v>
+      </c>
+      <c r="G58" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="35">
         <v>53</v>
       </c>
@@ -9698,8 +10037,14 @@
       <c r="E59" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" s="51">
+        <v>10</v>
+      </c>
+      <c r="G59" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="35">
         <v>54</v>
       </c>
@@ -9713,8 +10058,14 @@
       <c r="E60" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" s="51">
+        <v>8</v>
+      </c>
+      <c r="G60" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="35">
         <v>55</v>
       </c>
@@ -9728,8 +10079,14 @@
       <c r="E61" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" s="51">
+        <v>7</v>
+      </c>
+      <c r="G61" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="35">
         <v>56</v>
       </c>
@@ -9743,8 +10100,14 @@
       <c r="E62" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="51">
+        <v>8</v>
+      </c>
+      <c r="G62" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="35">
         <v>57</v>
       </c>
@@ -9760,8 +10123,14 @@
       <c r="E63" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" s="51">
+        <v>9</v>
+      </c>
+      <c r="G63" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="35">
         <v>58</v>
       </c>
@@ -9775,8 +10144,14 @@
       <c r="E64" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="51">
+        <v>10</v>
+      </c>
+      <c r="G64" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="35">
         <v>59</v>
       </c>
@@ -9792,8 +10167,14 @@
       <c r="E65" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="51">
+        <v>3</v>
+      </c>
+      <c r="G65" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="35">
         <v>60</v>
       </c>
@@ -9807,8 +10188,14 @@
       <c r="E66" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="51">
+        <v>6</v>
+      </c>
+      <c r="G66" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="35">
         <v>61</v>
       </c>
@@ -9822,8 +10209,14 @@
       <c r="E67" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" s="51">
+        <v>3</v>
+      </c>
+      <c r="G67" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="35">
         <v>62</v>
       </c>
@@ -9837,8 +10230,14 @@
       <c r="E68" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="51">
+        <v>9</v>
+      </c>
+      <c r="G68" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="35">
         <v>63</v>
       </c>
@@ -9852,8 +10251,14 @@
       <c r="E69" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="51">
+        <v>10</v>
+      </c>
+      <c r="G69" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="35">
         <v>64</v>
       </c>
@@ -9867,8 +10272,14 @@
       <c r="E70" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="51">
+        <v>12</v>
+      </c>
+      <c r="G70" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="35">
         <v>65</v>
       </c>
@@ -9884,8 +10295,14 @@
       <c r="E71" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" s="51">
+        <v>10</v>
+      </c>
+      <c r="G71" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="35">
         <v>66</v>
       </c>
@@ -9901,8 +10318,14 @@
       <c r="E72" s="36" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" s="51">
+        <v>2</v>
+      </c>
+      <c r="G72" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="35">
         <v>67</v>
       </c>
@@ -9918,8 +10341,14 @@
       <c r="E73" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="51">
+        <v>3</v>
+      </c>
+      <c r="G73" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="35">
         <v>68</v>
       </c>
@@ -9935,8 +10364,14 @@
       <c r="E74" s="36" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" s="51">
+        <v>10</v>
+      </c>
+      <c r="G74" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="35">
         <v>69</v>
       </c>
@@ -9952,8 +10387,14 @@
       <c r="E75" s="36" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" s="51">
+        <v>11</v>
+      </c>
+      <c r="G75" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="35">
         <v>70</v>
       </c>
@@ -9969,8 +10410,14 @@
       <c r="E76" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" s="51">
+        <v>12</v>
+      </c>
+      <c r="G76" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="35">
         <v>71</v>
       </c>
@@ -9986,15 +10433,21 @@
       <c r="E77" s="36" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" s="51">
+        <v>2</v>
+      </c>
+      <c r="G77" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="35"/>
       <c r="B78" s="36"/>
       <c r="C78" s="36"/>
       <c r="D78" s="36"/>
       <c r="E78" s="36"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="35">
         <v>72</v>
       </c>
@@ -10008,8 +10461,14 @@
       <c r="E79" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" s="51">
+        <v>3</v>
+      </c>
+      <c r="G79" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="35">
         <v>73</v>
       </c>
@@ -10023,8 +10482,14 @@
       <c r="E80" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80" s="51">
+        <v>12</v>
+      </c>
+      <c r="G80" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="35">
         <v>74</v>
       </c>
@@ -10038,8 +10503,14 @@
       <c r="E81" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81" s="51">
+        <v>12</v>
+      </c>
+      <c r="G81" s="51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="35">
         <v>75</v>
       </c>
@@ -10053,8 +10524,14 @@
       <c r="E82" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82" s="51">
+        <v>12</v>
+      </c>
+      <c r="G82" s="51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="35">
         <v>76</v>
       </c>
@@ -10068,8 +10545,14 @@
       <c r="E83" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83" s="51">
+        <v>10</v>
+      </c>
+      <c r="G83" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="35">
         <v>77</v>
       </c>
@@ -10083,8 +10566,14 @@
       <c r="E84" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84" s="51">
+        <v>12</v>
+      </c>
+      <c r="G84" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="35">
         <v>78</v>
       </c>
@@ -10098,8 +10587,14 @@
       <c r="E85" s="36" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85" s="51">
+        <v>12</v>
+      </c>
+      <c r="G85" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="35">
         <v>79</v>
       </c>
@@ -10113,8 +10608,14 @@
       <c r="E86" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86" s="51">
+        <v>12</v>
+      </c>
+      <c r="G86" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="35">
         <v>80</v>
       </c>
@@ -10128,8 +10629,14 @@
       <c r="E87" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" s="51">
+        <v>6</v>
+      </c>
+      <c r="G87" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="35">
         <v>81</v>
       </c>
@@ -10143,8 +10650,14 @@
       <c r="E88" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88" s="51">
+        <v>12</v>
+      </c>
+      <c r="G88" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="35">
         <v>82</v>
       </c>
@@ -10158,8 +10671,14 @@
       <c r="E89" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89" s="51">
+        <v>8</v>
+      </c>
+      <c r="G89" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="35">
         <v>83</v>
       </c>
@@ -10173,8 +10692,14 @@
       <c r="E90" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90" s="51">
+        <v>3</v>
+      </c>
+      <c r="G90" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="35">
         <v>84</v>
       </c>
@@ -10188,8 +10713,14 @@
       <c r="E91" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91" s="51">
+        <v>6</v>
+      </c>
+      <c r="G91" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="35">
         <v>85</v>
       </c>
@@ -10203,8 +10734,14 @@
       <c r="E92" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92" s="51">
+        <v>9</v>
+      </c>
+      <c r="G92" s="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="35">
         <v>86</v>
       </c>
@@ -10218,8 +10755,14 @@
       <c r="E93" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93" s="51">
+        <v>11</v>
+      </c>
+      <c r="G93" s="51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="35">
         <v>87</v>
       </c>
@@ -10233,8 +10776,14 @@
       <c r="E94" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94" s="51">
+        <v>9</v>
+      </c>
+      <c r="G94" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="35">
         <v>88</v>
       </c>
@@ -10248,8 +10797,14 @@
       <c r="E95" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95" s="51">
+        <v>8</v>
+      </c>
+      <c r="G95" s="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="35">
         <v>89</v>
       </c>
@@ -10263,8 +10818,14 @@
       <c r="E96" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96" s="51">
+        <v>8</v>
+      </c>
+      <c r="G96" s="51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="35">
         <v>90</v>
       </c>
@@ -10278,8 +10839,14 @@
       <c r="E97" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97" s="51">
+        <v>9</v>
+      </c>
+      <c r="G97" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="35">
         <v>91</v>
       </c>
@@ -10293,8 +10860,14 @@
       <c r="E98" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98" s="51">
+        <v>3</v>
+      </c>
+      <c r="G98" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="35">
         <v>92</v>
       </c>
@@ -10308,8 +10881,14 @@
       <c r="E99" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99" s="51">
+        <v>10</v>
+      </c>
+      <c r="G99" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="35">
         <v>93</v>
       </c>
@@ -10323,8 +10902,14 @@
       <c r="E100" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100" s="51">
+        <v>8</v>
+      </c>
+      <c r="G100" s="51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="35">
         <v>94</v>
       </c>
@@ -10338,8 +10923,14 @@
       <c r="E101" s="36" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101" s="51">
+        <v>11</v>
+      </c>
+      <c r="G101" s="51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="35">
         <v>95</v>
       </c>
@@ -10352,6 +10943,12 @@
       <c r="D102" s="36"/>
       <c r="E102" s="36" t="s">
         <v>341</v>
+      </c>
+      <c r="F102" s="51">
+        <v>7</v>
+      </c>
+      <c r="G102" s="51">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -10359,7 +10956,8 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:B3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated IBM 1620 Max keyboard layout.
</commit_message>
<xml_diff>
--- a/docs/wheelwriter/keyboard_matrix.xlsx
+++ b/docs/wheelwriter/keyboard_matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cygwin\home\Dave\github\Cadetwriter\docs\wheelwriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FB23D0-86A8-44E3-B77F-BE9217146A22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B547F58-5251-41CD-AC41-39C949C6EDEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5E82A069-CE49-40B7-9E46-07FE8FC3DAB8}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <sheet name="ASCII Keyboard" sheetId="10" r:id="rId8"/>
     <sheet name="IBM 1620 Max" sheetId="11" r:id="rId9"/>
     <sheet name="IBM 1620 Max Keyboard" sheetId="12" r:id="rId10"/>
-    <sheet name="Wheelwriter Printwheels" sheetId="15" r:id="rId11"/>
+    <sheet name="Printwheels" sheetId="15" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="6">ASCII!$A$1:$Q$13</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="526">
   <si>
     <t>KYBD-8
 J14-8</t>
@@ -5044,16 +5044,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">(76)
-FLG
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(69)
-R-S
-</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">(8)
 </t>
@@ -6845,6 +6835,28 @@
   </si>
   <si>
     <t>Row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(69)
+FLAG
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(72)
+R-S
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DEL</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -7369,6 +7381,22 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7378,10 +7406,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7394,20 +7418,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7903,20 +7915,20 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:colOff>346904</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>112192</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC9ABF1B-70D6-43FA-A48B-C7D185D3CDB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F158EF03-8AF4-488D-9C62-2B47FEE62611}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7938,8 +7950,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="10058400" cy="2779192"/>
+          <a:off x="0" y="466725"/>
+          <a:ext cx="10100504" cy="2790825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8253,9 +8265,7 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8266,31 +8276,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>319</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="A1" s="40" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -8340,7 +8350,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="45" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -8390,7 +8400,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -8503,7 +8513,7 @@
         <v>84</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
@@ -8799,10 +8809,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
@@ -8816,19 +8825,17 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>324</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="A1" s="40" t="s">
+        <v>322</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -8837,9 +8844,6 @@
       <c r="D2" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -8848,25 +8852,23 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA42E1F6-175A-4BE2-8B97-2ABE974B15A6}">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G102"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="7" width="9.140625" style="51"/>
+    <col min="6" max="7" width="9.140625" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
-        <v>335</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="A1" s="42" t="s">
+        <v>333</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -8876,24 +8878,24 @@
       <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="51" t="s">
+        <v>334</v>
+      </c>
+      <c r="B3" s="51"/>
+      <c r="C3" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="D3" s="37" t="s">
         <v>336</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="37" t="s">
+      <c r="E3" s="37" t="s">
         <v>337</v>
       </c>
-      <c r="D3" s="37" t="s">
-        <v>338</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>339</v>
-      </c>
-      <c r="F3" s="50" t="s">
-        <v>524</v>
-      </c>
-      <c r="G3" s="50" t="s">
-        <v>525</v>
+      <c r="F3" s="38" t="s">
+        <v>522</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -8901,19 +8903,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D4" s="36"/>
       <c r="E4" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F4" s="51">
+        <v>339</v>
+      </c>
+      <c r="F4" s="39">
         <v>3</v>
       </c>
-      <c r="G4" s="51">
+      <c r="G4" s="39">
         <v>7</v>
       </c>
     </row>
@@ -8925,16 +8927,16 @@
         <v>65</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F5" s="51">
+        <v>339</v>
+      </c>
+      <c r="F5" s="39">
         <v>9</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="39">
         <v>1</v>
       </c>
     </row>
@@ -8946,16 +8948,16 @@
         <v>66</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F6" s="51">
+        <v>339</v>
+      </c>
+      <c r="F6" s="39">
         <v>8</v>
       </c>
-      <c r="G6" s="51">
+      <c r="G6" s="39">
         <v>4</v>
       </c>
     </row>
@@ -8967,16 +8969,16 @@
         <v>67</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F7" s="51">
+        <v>339</v>
+      </c>
+      <c r="F7" s="39">
         <v>9</v>
       </c>
-      <c r="G7" s="51">
+      <c r="G7" s="39">
         <v>2</v>
       </c>
     </row>
@@ -8988,16 +8990,16 @@
         <v>68</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D8" s="36"/>
       <c r="E8" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F8" s="51">
+        <v>339</v>
+      </c>
+      <c r="F8" s="39">
         <v>7</v>
       </c>
-      <c r="G8" s="51">
+      <c r="G8" s="39">
         <v>2</v>
       </c>
     </row>
@@ -9009,16 +9011,16 @@
         <v>69</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D9" s="36"/>
       <c r="E9" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F9" s="51">
+        <v>339</v>
+      </c>
+      <c r="F9" s="39">
         <v>6</v>
       </c>
-      <c r="G9" s="51">
+      <c r="G9" s="39">
         <v>7</v>
       </c>
     </row>
@@ -9030,16 +9032,16 @@
         <v>70</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D10" s="36"/>
       <c r="E10" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F10" s="51">
+        <v>339</v>
+      </c>
+      <c r="F10" s="39">
         <v>7</v>
       </c>
-      <c r="G10" s="51">
+      <c r="G10" s="39">
         <v>7</v>
       </c>
     </row>
@@ -9051,16 +9053,16 @@
         <v>71</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F11" s="51">
+        <v>339</v>
+      </c>
+      <c r="F11" s="39">
         <v>9</v>
       </c>
-      <c r="G11" s="51">
+      <c r="G11" s="39">
         <v>8</v>
       </c>
     </row>
@@ -9072,16 +9074,16 @@
         <v>72</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F12" s="51">
+        <v>339</v>
+      </c>
+      <c r="F12" s="39">
         <v>11</v>
       </c>
-      <c r="G12" s="51">
+      <c r="G12" s="39">
         <v>7</v>
       </c>
     </row>
@@ -9090,19 +9092,19 @@
         <v>9</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D13" s="36"/>
       <c r="E13" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F13" s="51">
+        <v>339</v>
+      </c>
+      <c r="F13" s="39">
         <v>8</v>
       </c>
-      <c r="G13" s="51">
+      <c r="G13" s="39">
         <v>7</v>
       </c>
     </row>
@@ -9111,19 +9113,19 @@
         <v>10</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F14" s="51">
+        <v>339</v>
+      </c>
+      <c r="F14" s="39">
         <v>10</v>
       </c>
-      <c r="G14" s="51">
+      <c r="G14" s="39">
         <v>7</v>
       </c>
     </row>
@@ -9132,19 +9134,19 @@
         <v>11</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D15" s="36"/>
       <c r="E15" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F15" s="51">
+        <v>357</v>
+      </c>
+      <c r="F15" s="39">
         <v>10</v>
       </c>
-      <c r="G15" s="51">
+      <c r="G15" s="39">
         <v>2</v>
       </c>
     </row>
@@ -9153,19 +9155,19 @@
         <v>12</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D16" s="36"/>
       <c r="E16" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F16" s="51">
+        <v>357</v>
+      </c>
+      <c r="F16" s="39">
         <v>8</v>
       </c>
-      <c r="G16" s="51">
+      <c r="G16" s="39">
         <v>2</v>
       </c>
     </row>
@@ -9174,19 +9176,19 @@
         <v>13</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D17" s="36"/>
       <c r="E17" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F17" s="51">
+        <v>339</v>
+      </c>
+      <c r="F17" s="39">
         <v>12</v>
       </c>
-      <c r="G17" s="51">
+      <c r="G17" s="39">
         <v>6</v>
       </c>
     </row>
@@ -9195,19 +9197,19 @@
         <v>14</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D18" s="36"/>
       <c r="E18" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F18" s="51">
+        <v>357</v>
+      </c>
+      <c r="F18" s="39">
         <v>8</v>
       </c>
-      <c r="G18" s="51">
+      <c r="G18" s="39">
         <v>8</v>
       </c>
     </row>
@@ -9216,19 +9218,19 @@
         <v>15</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D19" s="36"/>
       <c r="E19" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F19" s="51">
+        <v>357</v>
+      </c>
+      <c r="F19" s="39">
         <v>9</v>
       </c>
-      <c r="G19" s="51">
+      <c r="G19" s="39">
         <v>4</v>
       </c>
     </row>
@@ -9237,19 +9239,19 @@
         <v>16</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D20" s="36"/>
       <c r="E20" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F20" s="51">
+        <v>357</v>
+      </c>
+      <c r="F20" s="39">
         <v>8</v>
       </c>
-      <c r="G20" s="51">
+      <c r="G20" s="39">
         <v>7</v>
       </c>
     </row>
@@ -9258,19 +9260,19 @@
         <v>17</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D21" s="36"/>
       <c r="E21" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F21" s="51">
+        <v>357</v>
+      </c>
+      <c r="F21" s="39">
         <v>8</v>
       </c>
-      <c r="G21" s="51">
+      <c r="G21" s="39">
         <v>1</v>
       </c>
     </row>
@@ -9279,19 +9281,19 @@
         <v>18</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D22" s="36"/>
       <c r="E22" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F22" s="51">
+        <v>357</v>
+      </c>
+      <c r="F22" s="39">
         <v>3</v>
       </c>
-      <c r="G22" s="51">
+      <c r="G22" s="39">
         <v>2</v>
       </c>
     </row>
@@ -9300,19 +9302,19 @@
         <v>19</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D23" s="36"/>
       <c r="E23" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F23" s="51">
+        <v>357</v>
+      </c>
+      <c r="F23" s="39">
         <v>9</v>
       </c>
-      <c r="G23" s="51">
+      <c r="G23" s="39">
         <v>8</v>
       </c>
     </row>
@@ -9321,19 +9323,19 @@
         <v>20</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D24" s="36"/>
       <c r="E24" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F24" s="51">
+        <v>357</v>
+      </c>
+      <c r="F24" s="39">
         <v>12</v>
       </c>
-      <c r="G24" s="51">
+      <c r="G24" s="39">
         <v>4</v>
       </c>
     </row>
@@ -9342,19 +9344,19 @@
         <v>21</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D25" s="36"/>
       <c r="E25" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F25" s="51">
+        <v>357</v>
+      </c>
+      <c r="F25" s="39">
         <v>12</v>
       </c>
-      <c r="G25" s="51">
+      <c r="G25" s="39">
         <v>5</v>
       </c>
     </row>
@@ -9363,19 +9365,19 @@
         <v>22</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D26" s="36"/>
       <c r="E26" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F26" s="51">
+        <v>357</v>
+      </c>
+      <c r="F26" s="39">
         <v>8</v>
       </c>
-      <c r="G26" s="51">
+      <c r="G26" s="39">
         <v>4</v>
       </c>
     </row>
@@ -9384,19 +9386,19 @@
         <v>23</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D27" s="36"/>
       <c r="E27" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F27" s="51">
+        <v>357</v>
+      </c>
+      <c r="F27" s="39">
         <v>11</v>
       </c>
-      <c r="G27" s="51">
+      <c r="G27" s="39">
         <v>7</v>
       </c>
     </row>
@@ -9412,19 +9414,19 @@
         <v>24</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D29" s="36"/>
       <c r="E29" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F29" s="51">
+        <v>357</v>
+      </c>
+      <c r="F29" s="39">
         <v>6</v>
       </c>
-      <c r="G29" s="51">
+      <c r="G29" s="39">
         <v>7</v>
       </c>
     </row>
@@ -9433,19 +9435,19 @@
         <v>25</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C30" s="36" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D30" s="36"/>
       <c r="E30" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F30" s="51">
+        <v>357</v>
+      </c>
+      <c r="F30" s="39">
         <v>9</v>
       </c>
-      <c r="G30" s="51">
+      <c r="G30" s="39">
         <v>1</v>
       </c>
     </row>
@@ -9454,19 +9456,19 @@
         <v>26</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D31" s="36"/>
       <c r="E31" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F31" s="51">
+        <v>357</v>
+      </c>
+      <c r="F31" s="39">
         <v>7</v>
       </c>
-      <c r="G31" s="51">
+      <c r="G31" s="39">
         <v>2</v>
       </c>
     </row>
@@ -9475,19 +9477,19 @@
         <v>27</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D32" s="36"/>
       <c r="E32" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F32" s="51">
+        <v>357</v>
+      </c>
+      <c r="F32" s="39">
         <v>8</v>
       </c>
-      <c r="G32" s="51">
+      <c r="G32" s="39">
         <v>3</v>
       </c>
     </row>
@@ -9496,19 +9498,19 @@
         <v>28</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C33" s="36" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D33" s="36"/>
       <c r="E33" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F33" s="51">
+        <v>357</v>
+      </c>
+      <c r="F33" s="39">
         <v>7</v>
       </c>
-      <c r="G33" s="51">
+      <c r="G33" s="39">
         <v>7</v>
       </c>
     </row>
@@ -9517,19 +9519,19 @@
         <v>29</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C34" s="36" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D34" s="36"/>
       <c r="E34" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F34" s="51">
+        <v>357</v>
+      </c>
+      <c r="F34" s="39">
         <v>7</v>
       </c>
-      <c r="G34" s="51">
+      <c r="G34" s="39">
         <v>4</v>
       </c>
     </row>
@@ -9538,19 +9540,19 @@
         <v>30</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D35" s="36"/>
       <c r="E35" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F35" s="51">
+        <v>357</v>
+      </c>
+      <c r="F35" s="39">
         <v>10</v>
       </c>
-      <c r="G35" s="51">
+      <c r="G35" s="39">
         <v>4</v>
       </c>
     </row>
@@ -9559,19 +9561,19 @@
         <v>31</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D36" s="36"/>
       <c r="E36" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F36" s="51">
+        <v>357</v>
+      </c>
+      <c r="F36" s="39">
         <v>3</v>
       </c>
-      <c r="G36" s="51">
+      <c r="G36" s="39">
         <v>7</v>
       </c>
     </row>
@@ -9580,19 +9582,19 @@
         <v>32</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D37" s="36"/>
       <c r="E37" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F37" s="51">
+        <v>357</v>
+      </c>
+      <c r="F37" s="39">
         <v>9</v>
       </c>
-      <c r="G37" s="51">
+      <c r="G37" s="39">
         <v>7</v>
       </c>
     </row>
@@ -9601,19 +9603,19 @@
         <v>33</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D38" s="36"/>
       <c r="E38" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F38" s="51">
+        <v>357</v>
+      </c>
+      <c r="F38" s="39">
         <v>11</v>
       </c>
-      <c r="G38" s="51">
+      <c r="G38" s="39">
         <v>4</v>
       </c>
     </row>
@@ -9622,19 +9624,19 @@
         <v>34</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D39" s="36"/>
       <c r="E39" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F39" s="51">
+        <v>357</v>
+      </c>
+      <c r="F39" s="39">
         <v>11</v>
       </c>
-      <c r="G39" s="51">
+      <c r="G39" s="39">
         <v>5</v>
       </c>
     </row>
@@ -9643,19 +9645,19 @@
         <v>35</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D40" s="36"/>
       <c r="E40" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F40" s="51">
+        <v>357</v>
+      </c>
+      <c r="F40" s="39">
         <v>9</v>
       </c>
-      <c r="G40" s="51">
+      <c r="G40" s="39">
         <v>2</v>
       </c>
     </row>
@@ -9664,19 +9666,19 @@
         <v>36</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D41" s="36"/>
       <c r="E41" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F41" s="51">
+        <v>339</v>
+      </c>
+      <c r="F41" s="39">
         <v>11</v>
       </c>
-      <c r="G41" s="51">
+      <c r="G41" s="39">
         <v>2</v>
       </c>
     </row>
@@ -9685,19 +9687,19 @@
         <v>37</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D42" s="36"/>
       <c r="E42" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F42" s="51">
+        <v>357</v>
+      </c>
+      <c r="F42" s="39">
         <v>9</v>
       </c>
-      <c r="G42" s="51">
+      <c r="G42" s="39">
         <v>3</v>
       </c>
     </row>
@@ -9706,19 +9708,19 @@
         <v>38</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D43" s="36"/>
       <c r="E43" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F43" s="51">
+        <v>339</v>
+      </c>
+      <c r="F43" s="39">
         <v>10</v>
       </c>
-      <c r="G43" s="51">
+      <c r="G43" s="39">
         <v>2</v>
       </c>
     </row>
@@ -9727,19 +9729,19 @@
         <v>39</v>
       </c>
       <c r="B44" s="36" t="s">
+        <v>408</v>
+      </c>
+      <c r="C44" s="36" t="s">
         <v>410</v>
-      </c>
-      <c r="C44" s="36" t="s">
-        <v>412</v>
       </c>
       <c r="D44" s="36"/>
       <c r="E44" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F44" s="51">
+        <v>339</v>
+      </c>
+      <c r="F44" s="39">
         <v>12</v>
       </c>
-      <c r="G44" s="51">
+      <c r="G44" s="39">
         <v>1</v>
       </c>
     </row>
@@ -9748,19 +9750,19 @@
         <v>40</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D45" s="36"/>
       <c r="E45" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F45" s="51">
+        <v>357</v>
+      </c>
+      <c r="F45" s="39">
         <v>6</v>
       </c>
-      <c r="G45" s="51">
+      <c r="G45" s="39">
         <v>4</v>
       </c>
     </row>
@@ -9769,19 +9771,19 @@
         <v>41</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C46" s="36">
         <v>9</v>
       </c>
       <c r="D46" s="36"/>
       <c r="E46" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F46" s="51">
+        <v>339</v>
+      </c>
+      <c r="F46" s="39">
         <v>11</v>
       </c>
-      <c r="G46" s="51">
+      <c r="G46" s="39">
         <v>5</v>
       </c>
     </row>
@@ -9790,19 +9792,19 @@
         <v>42</v>
       </c>
       <c r="B47" s="36" t="s">
+        <v>413</v>
+      </c>
+      <c r="C47" s="36" t="s">
         <v>415</v>
-      </c>
-      <c r="C47" s="36" t="s">
-        <v>417</v>
       </c>
       <c r="D47" s="36"/>
       <c r="E47" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F47" s="51">
+        <v>357</v>
+      </c>
+      <c r="F47" s="39">
         <v>10</v>
       </c>
-      <c r="G47" s="51">
+      <c r="G47" s="39">
         <v>7</v>
       </c>
     </row>
@@ -9811,19 +9813,19 @@
         <v>43</v>
       </c>
       <c r="B48" s="36" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C48" s="36">
         <v>3</v>
       </c>
       <c r="D48" s="36"/>
       <c r="E48" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F48" s="51">
+        <v>339</v>
+      </c>
+      <c r="F48" s="39">
         <v>7</v>
       </c>
-      <c r="G48" s="51">
+      <c r="G48" s="39">
         <v>5</v>
       </c>
     </row>
@@ -9832,19 +9834,19 @@
         <v>44</v>
       </c>
       <c r="B49" s="36" t="s">
+        <v>416</v>
+      </c>
+      <c r="C49" s="36" t="s">
         <v>418</v>
-      </c>
-      <c r="C49" s="36" t="s">
-        <v>420</v>
       </c>
       <c r="D49" s="36"/>
       <c r="E49" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F49" s="51">
+        <v>357</v>
+      </c>
+      <c r="F49" s="39">
         <v>6</v>
       </c>
-      <c r="G49" s="51">
+      <c r="G49" s="39">
         <v>2</v>
       </c>
     </row>
@@ -9853,19 +9855,19 @@
         <v>45</v>
       </c>
       <c r="B50" s="36" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C50" s="36">
         <v>1</v>
       </c>
       <c r="D50" s="36"/>
       <c r="E50" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F50" s="51">
+        <v>339</v>
+      </c>
+      <c r="F50" s="39">
         <v>3</v>
       </c>
-      <c r="G50" s="51">
+      <c r="G50" s="39">
         <v>5</v>
       </c>
     </row>
@@ -9874,19 +9876,19 @@
         <v>46</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C51" s="36">
         <v>2</v>
       </c>
       <c r="D51" s="36"/>
       <c r="E51" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F51" s="51">
+        <v>339</v>
+      </c>
+      <c r="F51" s="39">
         <v>6</v>
       </c>
-      <c r="G51" s="51">
+      <c r="G51" s="39">
         <v>5</v>
       </c>
     </row>
@@ -9895,19 +9897,19 @@
         <v>47</v>
       </c>
       <c r="B52" s="36" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C52" s="36">
         <v>0</v>
       </c>
       <c r="D52" s="36"/>
       <c r="E52" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F52" s="51">
+        <v>339</v>
+      </c>
+      <c r="F52" s="39">
         <v>12</v>
       </c>
-      <c r="G52" s="51">
+      <c r="G52" s="39">
         <v>5</v>
       </c>
     </row>
@@ -9923,19 +9925,19 @@
         <v>48</v>
       </c>
       <c r="B54" s="36" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C54" s="36">
         <v>5</v>
       </c>
       <c r="D54" s="36"/>
       <c r="E54" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F54" s="51">
+        <v>339</v>
+      </c>
+      <c r="F54" s="39">
         <v>8</v>
       </c>
-      <c r="G54" s="51">
+      <c r="G54" s="39">
         <v>6</v>
       </c>
     </row>
@@ -9944,19 +9946,19 @@
         <v>49</v>
       </c>
       <c r="B55" s="36" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C55" s="36">
         <v>4</v>
       </c>
       <c r="D55" s="36"/>
       <c r="E55" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F55" s="51">
+        <v>339</v>
+      </c>
+      <c r="F55" s="39">
         <v>8</v>
       </c>
-      <c r="G55" s="51">
+      <c r="G55" s="39">
         <v>5</v>
       </c>
     </row>
@@ -9965,19 +9967,19 @@
         <v>50</v>
       </c>
       <c r="B56" s="36" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C56" s="36">
         <v>6</v>
       </c>
       <c r="D56" s="36"/>
       <c r="E56" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F56" s="51">
+        <v>339</v>
+      </c>
+      <c r="F56" s="39">
         <v>9</v>
       </c>
-      <c r="G56" s="51">
+      <c r="G56" s="39">
         <v>6</v>
       </c>
     </row>
@@ -9986,19 +9988,19 @@
         <v>51</v>
       </c>
       <c r="B57" s="36" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C57" s="36">
         <v>8</v>
       </c>
       <c r="D57" s="36"/>
       <c r="E57" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F57" s="51">
+        <v>339</v>
+      </c>
+      <c r="F57" s="39">
         <v>10</v>
       </c>
-      <c r="G57" s="51">
+      <c r="G57" s="39">
         <v>5</v>
       </c>
     </row>
@@ -10007,19 +10009,19 @@
         <v>52</v>
       </c>
       <c r="B58" s="36" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C58" s="36">
         <v>7</v>
       </c>
       <c r="D58" s="36"/>
       <c r="E58" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F58" s="51">
+        <v>339</v>
+      </c>
+      <c r="F58" s="39">
         <v>9</v>
       </c>
-      <c r="G58" s="51">
+      <c r="G58" s="39">
         <v>5</v>
       </c>
     </row>
@@ -10028,19 +10030,19 @@
         <v>53</v>
       </c>
       <c r="B59" s="36" t="s">
+        <v>426</v>
+      </c>
+      <c r="C59" s="36" t="s">
         <v>428</v>
-      </c>
-      <c r="C59" s="36" t="s">
-        <v>430</v>
       </c>
       <c r="D59" s="36"/>
       <c r="E59" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F59" s="51">
+        <v>357</v>
+      </c>
+      <c r="F59" s="39">
         <v>10</v>
       </c>
-      <c r="G59" s="51">
+      <c r="G59" s="39">
         <v>5</v>
       </c>
     </row>
@@ -10049,19 +10051,19 @@
         <v>54</v>
       </c>
       <c r="B60" s="36" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C60" s="36" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D60" s="36"/>
       <c r="E60" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F60" s="51">
+        <v>357</v>
+      </c>
+      <c r="F60" s="39">
         <v>8</v>
       </c>
-      <c r="G60" s="51">
+      <c r="G60" s="39">
         <v>5</v>
       </c>
     </row>
@@ -10070,19 +10072,19 @@
         <v>55</v>
       </c>
       <c r="B61" s="36" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C61" s="36" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D61" s="36"/>
       <c r="E61" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F61" s="51">
+        <v>357</v>
+      </c>
+      <c r="F61" s="39">
         <v>7</v>
       </c>
-      <c r="G61" s="51">
+      <c r="G61" s="39">
         <v>5</v>
       </c>
     </row>
@@ -10091,19 +10093,19 @@
         <v>56</v>
       </c>
       <c r="B62" s="36" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C62" s="36" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D62" s="36"/>
       <c r="E62" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F62" s="51">
+        <v>357</v>
+      </c>
+      <c r="F62" s="39">
         <v>8</v>
       </c>
-      <c r="G62" s="51">
+      <c r="G62" s="39">
         <v>6</v>
       </c>
     </row>
@@ -10112,21 +10114,21 @@
         <v>57</v>
       </c>
       <c r="B63" s="36" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C63" s="36" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D63" s="36" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E63" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F63" s="51">
+        <v>357</v>
+      </c>
+      <c r="F63" s="39">
         <v>9</v>
       </c>
-      <c r="G63" s="51">
+      <c r="G63" s="39">
         <v>6</v>
       </c>
     </row>
@@ -10135,357 +10137,360 @@
         <v>58</v>
       </c>
       <c r="B64" s="36" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C64" s="36" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D64" s="36"/>
       <c r="E64" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F64" s="51">
+        <v>357</v>
+      </c>
+      <c r="F64" s="39">
         <v>10</v>
       </c>
-      <c r="G64" s="51">
+      <c r="G64" s="39">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="35">
         <v>59</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C65" s="36" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D65" s="36" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E65" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F65" s="51">
+        <v>339</v>
+      </c>
+      <c r="F65" s="39">
         <v>3</v>
       </c>
-      <c r="G65" s="51">
+      <c r="G65" s="39">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="35">
         <v>60</v>
       </c>
       <c r="B66" s="36" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C66" s="36" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D66" s="36"/>
       <c r="E66" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F66" s="51">
+        <v>357</v>
+      </c>
+      <c r="F66" s="39">
         <v>6</v>
       </c>
-      <c r="G66" s="51">
+      <c r="G66" s="39">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="35">
         <v>61</v>
       </c>
       <c r="B67" s="36" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C67" s="36" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D67" s="36"/>
       <c r="E67" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F67" s="51">
+        <v>357</v>
+      </c>
+      <c r="F67" s="39">
         <v>3</v>
       </c>
-      <c r="G67" s="51">
+      <c r="G67" s="39">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="35">
         <v>62</v>
       </c>
       <c r="B68" s="36" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C68" s="36" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D68" s="36"/>
       <c r="E68" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F68" s="51">
+        <v>357</v>
+      </c>
+      <c r="F68" s="39">
         <v>9</v>
       </c>
-      <c r="G68" s="51">
+      <c r="G68" s="39">
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="35">
         <v>63</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C69" s="36" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D69" s="36"/>
       <c r="E69" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F69" s="51">
+        <v>339</v>
+      </c>
+      <c r="F69" s="39">
         <v>10</v>
       </c>
-      <c r="G69" s="51">
+      <c r="G69" s="39">
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="35">
         <v>64</v>
       </c>
       <c r="B70" s="36" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C70" s="36" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D70" s="36"/>
       <c r="E70" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F70" s="51">
-        <v>12</v>
-      </c>
-      <c r="G70" s="51">
+        <v>357</v>
+      </c>
+      <c r="F70" s="39">
+        <v>10</v>
+      </c>
+      <c r="G70" s="39">
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="35">
         <v>65</v>
       </c>
       <c r="B71" s="36" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C71" s="36" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D71" s="36" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E71" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F71" s="51">
-        <v>10</v>
-      </c>
-      <c r="G71" s="51">
+        <v>459</v>
+      </c>
+      <c r="F71" s="39">
+        <v>12</v>
+      </c>
+      <c r="G71" s="39">
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="35">
         <v>66</v>
       </c>
       <c r="B72" s="36" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C72" s="36" t="s">
+        <v>457</v>
+      </c>
+      <c r="D72" s="36" t="s">
+        <v>458</v>
+      </c>
+      <c r="E72" s="36" t="s">
         <v>459</v>
       </c>
-      <c r="D72" s="36" t="s">
-        <v>460</v>
-      </c>
-      <c r="E72" s="36" t="s">
-        <v>461</v>
-      </c>
-      <c r="F72" s="51">
-        <v>2</v>
-      </c>
-      <c r="G72" s="51">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F72" s="39">
+        <v>10</v>
+      </c>
+      <c r="G72" s="39">
+        <v>3</v>
+      </c>
+      <c r="H72" s="36"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="35">
         <v>67</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C73" s="36" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D73" s="36" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="E73" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F73" s="51">
+        <v>357</v>
+      </c>
+      <c r="F73" s="39">
         <v>3</v>
       </c>
-      <c r="G73" s="51">
+      <c r="G73" s="39">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="35">
         <v>68</v>
       </c>
       <c r="B74" s="36" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C74" s="36" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D74" s="36" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="E74" s="36" t="s">
-        <v>461</v>
-      </c>
-      <c r="F74" s="51">
-        <v>10</v>
-      </c>
-      <c r="G74" s="51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+      <c r="F74" s="39">
+        <v>12</v>
+      </c>
+      <c r="G74" s="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="35">
         <v>69</v>
       </c>
       <c r="B75" s="36" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C75" s="36" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D75" s="36" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="E75" s="36" t="s">
-        <v>461</v>
-      </c>
-      <c r="F75" s="51">
-        <v>11</v>
-      </c>
-      <c r="G75" s="51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+      <c r="F75" s="39">
+        <v>12</v>
+      </c>
+      <c r="G75" s="39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="35">
         <v>70</v>
       </c>
       <c r="B76" s="36" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C76" s="36" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D76" s="36" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="E76" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F76" s="51">
+        <v>339</v>
+      </c>
+      <c r="F76" s="39">
         <v>12</v>
       </c>
-      <c r="G76" s="51">
+      <c r="G76" s="39">
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="35">
         <v>71</v>
       </c>
       <c r="B77" s="36" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C77" s="36" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D77" s="36" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E77" s="36" t="s">
-        <v>461</v>
-      </c>
-      <c r="F77" s="51">
-        <v>2</v>
-      </c>
-      <c r="G77" s="51">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+      <c r="F77" s="39">
+        <v>12</v>
+      </c>
+      <c r="G77" s="39">
+        <v>3</v>
+      </c>
+      <c r="H77" s="36"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="35"/>
       <c r="B78" s="36"/>
       <c r="C78" s="36"/>
       <c r="D78" s="36"/>
       <c r="E78" s="36"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78" s="36"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="35">
         <v>72</v>
       </c>
       <c r="B79" s="36" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C79" s="36" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D79" s="36"/>
       <c r="E79" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F79" s="51">
+        <v>357</v>
+      </c>
+      <c r="F79" s="39">
         <v>3</v>
       </c>
-      <c r="G79" s="51">
+      <c r="G79" s="39">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="35">
         <v>73</v>
       </c>
       <c r="B80" s="36" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C80" s="36" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D80" s="36"/>
       <c r="E80" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F80" s="51">
+        <v>357</v>
+      </c>
+      <c r="F80" s="39">
         <v>12</v>
       </c>
-      <c r="G80" s="51">
+      <c r="G80" s="39">
         <v>1</v>
       </c>
     </row>
@@ -10494,19 +10499,19 @@
         <v>74</v>
       </c>
       <c r="B81" s="36" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C81" s="36" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D81" s="36"/>
       <c r="E81" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F81" s="51">
+        <v>357</v>
+      </c>
+      <c r="F81" s="39">
         <v>12</v>
       </c>
-      <c r="G81" s="51">
+      <c r="G81" s="39">
         <v>8</v>
       </c>
     </row>
@@ -10515,19 +10520,19 @@
         <v>75</v>
       </c>
       <c r="B82" s="36" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C82" s="36" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D82" s="36"/>
       <c r="E82" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F82" s="51">
+        <v>339</v>
+      </c>
+      <c r="F82" s="39">
         <v>12</v>
       </c>
-      <c r="G82" s="51">
+      <c r="G82" s="39">
         <v>8</v>
       </c>
     </row>
@@ -10536,19 +10541,19 @@
         <v>76</v>
       </c>
       <c r="B83" s="36" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C83" s="36" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D83" s="36"/>
       <c r="E83" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F83" s="51">
+        <v>339</v>
+      </c>
+      <c r="F83" s="39">
         <v>10</v>
       </c>
-      <c r="G83" s="51">
+      <c r="G83" s="39">
         <v>6</v>
       </c>
     </row>
@@ -10557,19 +10562,19 @@
         <v>77</v>
       </c>
       <c r="B84" s="36" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C84" s="36" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D84" s="36"/>
       <c r="E84" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F84" s="51">
+        <v>357</v>
+      </c>
+      <c r="F84" s="39">
         <v>12</v>
       </c>
-      <c r="G84" s="51">
+      <c r="G84" s="39">
         <v>7</v>
       </c>
     </row>
@@ -10578,19 +10583,19 @@
         <v>78</v>
       </c>
       <c r="B85" s="36" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C85" s="36" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D85" s="36"/>
       <c r="E85" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F85" s="51">
+        <v>357</v>
+      </c>
+      <c r="F85" s="39">
         <v>12</v>
       </c>
-      <c r="G85" s="51">
+      <c r="G85" s="39">
         <v>6</v>
       </c>
     </row>
@@ -10599,19 +10604,19 @@
         <v>79</v>
       </c>
       <c r="B86" s="36" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C86" s="36" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D86" s="36"/>
       <c r="E86" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F86" s="51">
+        <v>339</v>
+      </c>
+      <c r="F86" s="39">
         <v>12</v>
       </c>
-      <c r="G86" s="51">
+      <c r="G86" s="39">
         <v>7</v>
       </c>
     </row>
@@ -10620,19 +10625,19 @@
         <v>80</v>
       </c>
       <c r="B87" s="36" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C87" s="36" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D87" s="36"/>
       <c r="E87" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F87" s="51">
+        <v>339</v>
+      </c>
+      <c r="F87" s="39">
         <v>6</v>
       </c>
-      <c r="G87" s="51">
+      <c r="G87" s="39">
         <v>2</v>
       </c>
     </row>
@@ -10641,19 +10646,19 @@
         <v>81</v>
       </c>
       <c r="B88" s="36" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C88" s="36" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D88" s="36"/>
       <c r="E88" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F88" s="51">
+        <v>339</v>
+      </c>
+      <c r="F88" s="39">
         <v>12</v>
       </c>
-      <c r="G88" s="51">
+      <c r="G88" s="39">
         <v>4</v>
       </c>
     </row>
@@ -10662,19 +10667,19 @@
         <v>82</v>
       </c>
       <c r="B89" s="36" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C89" s="36" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D89" s="36"/>
       <c r="E89" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F89" s="51">
+        <v>339</v>
+      </c>
+      <c r="F89" s="39">
         <v>8</v>
       </c>
-      <c r="G89" s="51">
+      <c r="G89" s="39">
         <v>2</v>
       </c>
     </row>
@@ -10683,19 +10688,19 @@
         <v>83</v>
       </c>
       <c r="B90" s="36" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C90" s="36" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D90" s="36"/>
       <c r="E90" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F90" s="51">
+        <v>339</v>
+      </c>
+      <c r="F90" s="39">
         <v>3</v>
       </c>
-      <c r="G90" s="51">
+      <c r="G90" s="39">
         <v>2</v>
       </c>
     </row>
@@ -10704,19 +10709,19 @@
         <v>84</v>
       </c>
       <c r="B91" s="36" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C91" s="36" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D91" s="36"/>
       <c r="E91" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F91" s="51">
+        <v>339</v>
+      </c>
+      <c r="F91" s="39">
         <v>6</v>
       </c>
-      <c r="G91" s="51">
+      <c r="G91" s="39">
         <v>4</v>
       </c>
     </row>
@@ -10725,19 +10730,19 @@
         <v>85</v>
       </c>
       <c r="B92" s="36" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C92" s="36" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D92" s="36"/>
       <c r="E92" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F92" s="51">
+        <v>339</v>
+      </c>
+      <c r="F92" s="39">
         <v>9</v>
       </c>
-      <c r="G92" s="51">
+      <c r="G92" s="39">
         <v>7</v>
       </c>
     </row>
@@ -10746,19 +10751,19 @@
         <v>86</v>
       </c>
       <c r="B93" s="36" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C93" s="36" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D93" s="36"/>
       <c r="E93" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F93" s="51">
+        <v>357</v>
+      </c>
+      <c r="F93" s="39">
         <v>11</v>
       </c>
-      <c r="G93" s="51">
+      <c r="G93" s="39">
         <v>2</v>
       </c>
     </row>
@@ -10767,19 +10772,19 @@
         <v>87</v>
       </c>
       <c r="B94" s="36" t="s">
+        <v>503</v>
+      </c>
+      <c r="C94" s="36" t="s">
         <v>505</v>
-      </c>
-      <c r="C94" s="36" t="s">
-        <v>507</v>
       </c>
       <c r="D94" s="36"/>
       <c r="E94" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F94" s="51">
+        <v>339</v>
+      </c>
+      <c r="F94" s="39">
         <v>9</v>
       </c>
-      <c r="G94" s="51">
+      <c r="G94" s="39">
         <v>3</v>
       </c>
     </row>
@@ -10788,19 +10793,19 @@
         <v>88</v>
       </c>
       <c r="B95" s="36" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C95" s="36" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D95" s="36"/>
       <c r="E95" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F95" s="51">
+        <v>339</v>
+      </c>
+      <c r="F95" s="39">
         <v>8</v>
       </c>
-      <c r="G95" s="51">
+      <c r="G95" s="39">
         <v>1</v>
       </c>
     </row>
@@ -10809,19 +10814,19 @@
         <v>89</v>
       </c>
       <c r="B96" s="36" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C96" s="36" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D96" s="36"/>
       <c r="E96" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F96" s="51">
+        <v>339</v>
+      </c>
+      <c r="F96" s="39">
         <v>8</v>
       </c>
-      <c r="G96" s="51">
+      <c r="G96" s="39">
         <v>8</v>
       </c>
     </row>
@@ -10830,19 +10835,19 @@
         <v>90</v>
       </c>
       <c r="B97" s="36" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C97" s="36" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D97" s="36"/>
       <c r="E97" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F97" s="51">
+        <v>339</v>
+      </c>
+      <c r="F97" s="39">
         <v>9</v>
       </c>
-      <c r="G97" s="51">
+      <c r="G97" s="39">
         <v>4</v>
       </c>
     </row>
@@ -10851,19 +10856,19 @@
         <v>91</v>
       </c>
       <c r="B98" s="36" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C98" s="36" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D98" s="36"/>
       <c r="E98" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F98" s="51">
+        <v>339</v>
+      </c>
+      <c r="F98" s="39">
         <v>3</v>
       </c>
-      <c r="G98" s="51">
+      <c r="G98" s="39">
         <v>4</v>
       </c>
     </row>
@@ -10872,19 +10877,19 @@
         <v>92</v>
       </c>
       <c r="B99" s="36" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C99" s="36" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D99" s="36"/>
       <c r="E99" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F99" s="51">
+        <v>339</v>
+      </c>
+      <c r="F99" s="39">
         <v>10</v>
       </c>
-      <c r="G99" s="51">
+      <c r="G99" s="39">
         <v>4</v>
       </c>
     </row>
@@ -10893,19 +10898,19 @@
         <v>93</v>
       </c>
       <c r="B100" s="36" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C100" s="36" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D100" s="36"/>
       <c r="E100" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F100" s="51">
+        <v>339</v>
+      </c>
+      <c r="F100" s="39">
         <v>8</v>
       </c>
-      <c r="G100" s="51">
+      <c r="G100" s="39">
         <v>3</v>
       </c>
     </row>
@@ -10914,19 +10919,19 @@
         <v>94</v>
       </c>
       <c r="B101" s="36" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C101" s="36" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D101" s="36"/>
       <c r="E101" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F101" s="51">
+        <v>339</v>
+      </c>
+      <c r="F101" s="39">
         <v>11</v>
       </c>
-      <c r="G101" s="51">
+      <c r="G101" s="39">
         <v>4</v>
       </c>
     </row>
@@ -10935,25 +10940,48 @@
         <v>95</v>
       </c>
       <c r="B102" s="36" t="s">
+        <v>518</v>
+      </c>
+      <c r="C102" s="36" t="s">
         <v>520</v>
-      </c>
-      <c r="C102" s="36" t="s">
-        <v>522</v>
       </c>
       <c r="D102" s="36"/>
       <c r="E102" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F102" s="51">
+        <v>339</v>
+      </c>
+      <c r="F102" s="39">
         <v>7</v>
       </c>
-      <c r="G102" s="51">
+      <c r="G102" s="39">
         <v>4</v>
       </c>
     </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="35"/>
+      <c r="B103" s="36"/>
+      <c r="C103" s="36"/>
+      <c r="D103" s="36"/>
+      <c r="E103" s="36"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="35"/>
+      <c r="B104" s="36"/>
+      <c r="C104" s="36"/>
+      <c r="D104" s="36"/>
+      <c r="E104" s="36"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="35"/>
+      <c r="B105" s="36"/>
+      <c r="C105" s="36"/>
+      <c r="D105" s="36"/>
+      <c r="E105" s="36"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:H102">
+    <sortCondition ref="A4:A102"/>
+  </sortState>
+  <mergeCells count="1">
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10975,12 +11003,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>320</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="A1" s="40" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -10989,9 +11017,6 @@
       <c r="D2" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -11018,31 +11043,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>285</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="A1" s="40" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="38" t="s">
-        <v>286</v>
-      </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
+      <c r="D2" s="44" t="s">
+        <v>284</v>
+      </c>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -11092,57 +11117,57 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="45" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>300</v>
-      </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="32" t="s">
         <v>63</v>
       </c>
@@ -11197,7 +11222,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>65</v>
@@ -11240,7 +11265,7 @@
         <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>66</v>
@@ -11255,7 +11280,7 @@
         <v>84</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
@@ -11289,7 +11314,7 @@
         <v>73</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>67</v>
@@ -11300,7 +11325,7 @@
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="33" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -11328,7 +11353,7 @@
         <v>74</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>68</v>
@@ -11348,7 +11373,7 @@
         <v>113</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="K9" s="22" t="s">
         <v>123</v>
@@ -11363,10 +11388,10 @@
         <v>143</v>
       </c>
       <c r="O9" s="22" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="P9" s="33" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="Q9" s="24" t="s">
         <v>163</v>
@@ -11377,7 +11402,7 @@
         <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>69</v>
@@ -11390,7 +11415,7 @@
         <v>86</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="22" t="s">
@@ -11412,10 +11437,10 @@
         <v>144</v>
       </c>
       <c r="O10" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="P10" s="33" t="s">
         <v>330</v>
-      </c>
-      <c r="P10" s="33" t="s">
-        <v>332</v>
       </c>
       <c r="Q10" s="15"/>
     </row>
@@ -11424,7 +11449,7 @@
         <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>70</v>
@@ -11437,7 +11462,7 @@
         <v>87</v>
       </c>
       <c r="G11" s="33" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
@@ -11459,7 +11484,7 @@
         <v>157</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -11467,7 +11492,7 @@
         <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>71</v>
@@ -11480,7 +11505,7 @@
         <v>88</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="22" t="s">
@@ -11490,10 +11515,10 @@
         <v>119</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="M12" s="22" t="s">
         <v>141</v>
@@ -11505,10 +11530,10 @@
         <v>151</v>
       </c>
       <c r="P12" s="33" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="Q12" s="24" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -11516,7 +11541,7 @@
         <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>72</v>
@@ -11527,7 +11552,7 @@
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="23" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
@@ -11547,32 +11572,31 @@
         <v>159</v>
       </c>
       <c r="Q13" s="34" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="43" t="s">
-        <v>317</v>
-      </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
+      <c r="B16" s="47" t="s">
+        <v>315</v>
+      </c>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49"/>
     </row>
     <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="46" t="s">
-        <v>318</v>
-      </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="45"/>
+      <c r="B18" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
@@ -11593,12 +11617,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>321</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="A1" s="40" t="s">
+        <v>319</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -11607,9 +11631,6 @@
       <c r="D2" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -11623,9 +11644,7 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11636,31 +11655,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>283</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="A1" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -11710,7 +11729,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="45" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -11760,7 +11779,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -11869,7 +11888,7 @@
         <v>104</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
@@ -12133,10 +12152,9 @@
       <c r="Q13" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="96" fitToWidth="0" orientation="landscape" r:id="rId1"/>
@@ -12157,12 +12175,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>322</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="A1" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -12171,9 +12189,6 @@
       <c r="D2" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -12200,29 +12215,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -12272,7 +12287,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="45" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -12322,7 +12337,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -12707,10 +12722,9 @@
       <c r="Q13" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="96" fitToWidth="0" orientation="landscape" r:id="rId1"/>
@@ -12731,11 +12745,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>323</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
+      <c r="A1" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
       <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12745,9 +12759,6 @@
       <c r="D2" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -12761,9 +12772,7 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12774,31 +12783,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>284</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
+      <c r="A1" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -12848,7 +12857,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="45" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -12898,7 +12907,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -12974,10 +12983,10 @@
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="21" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -12987,7 +12996,9 @@
       <c r="P6" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="Q6" s="27"/>
+      <c r="Q6" s="25" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -13004,23 +13015,23 @@
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>236</v>
@@ -13054,17 +13065,17 @@
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="22" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="22" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="24" t="s">
@@ -13083,35 +13094,35 @@
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="F9" s="22" t="s">
         <v>253</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>255</v>
       </c>
       <c r="G9" s="22" t="s">
         <v>106</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="22" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="N9" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="O9" s="22" t="s">
         <v>280</v>
-      </c>
-      <c r="O9" s="22" t="s">
-        <v>282</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="24" t="s">
@@ -13174,7 +13185,7 @@
         <v>92</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -13194,10 +13205,10 @@
         <v>150</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>251</v>
+        <v>524</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -13212,30 +13223,30 @@
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="22" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="22" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="O12" s="22" t="s">
         <v>246</v>
@@ -13267,10 +13278,10 @@
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="23" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
@@ -13283,10 +13294,9 @@
       <c r="Q13" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="96" fitToWidth="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Corrected mapping of margin and tab control keys.
</commit_message>
<xml_diff>
--- a/docs/wheelwriter/keyboard_matrix.xlsx
+++ b/docs/wheelwriter/keyboard_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cygwin\home\Dave\github\Cadetwriter\docs\wheelwriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5686262C-68F7-421C-8990-36F2F652DC3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A727F76-E0DD-47EE-997D-FBEF23974D08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5E82A069-CE49-40B7-9E46-07FE8FC3DAB8}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="587">
   <si>
     <t>KYBD-8
 J14-8</t>
@@ -2836,10 +2836,6 @@
     </r>
   </si>
   <si>
-    <t>(16)
-&lt;load paper&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">(24)
 X
 </t>
@@ -3446,34 +3442,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">(76)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mar Rel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">(23)
 </t>
     </r>
@@ -4650,11 +4618,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">(76)
-ESC
-</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">(8)
 </t>
@@ -5740,23 +5703,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">(16)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;load paper&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>Wheelwriter Printwheel Positions</t>
   </si>
   <si>
@@ -6411,9 +6357,6 @@
     <t>Operation</t>
   </si>
   <si>
-    <t>Wheelwriter [non-printing] Operations</t>
-  </si>
-  <si>
     <t>&lt;left shift&gt;</t>
   </si>
   <si>
@@ -7145,6 +7088,132 @@
   </si>
   <si>
     <t>Bksp 1</t>
+  </si>
+  <si>
+    <t>Wheelwriter [non-printing] Printer Operations</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(18)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L Mar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(74)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R Mar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(76)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mar Rel</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(77)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T Set</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(22)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;clear all&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>T Clr</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(76)
+ESC
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mar Rel</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -7695,17 +7764,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7732,8 +7794,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8579,7 +8648,9 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8590,31 +8661,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>301</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="A1" s="50" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -8664,7 +8735,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="43" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -8714,7 +8785,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -8827,7 +8898,7 @@
         <v>84</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
@@ -8884,11 +8955,11 @@
         <v>128</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="22" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="24" t="s">
@@ -8941,7 +9012,7 @@
         <v>148</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -9006,7 +9077,7 @@
         <v>80</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="G11" s="28" t="s">
         <v>106</v>
@@ -9018,7 +9089,7 @@
         <v>123</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="M11" s="22" t="s">
         <v>136</v>
@@ -9031,7 +9102,7 @@
         <v>150</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -9074,7 +9145,7 @@
         <v>141</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="P12" s="28" t="s">
         <v>151</v>
@@ -9113,7 +9184,7 @@
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="23" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="P13" s="23" t="s">
         <v>152</v>
@@ -9123,9 +9194,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="96" fitToWidth="0" orientation="landscape" r:id="rId1"/>
@@ -9139,17 +9211,19 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>306</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="A1" s="50" t="s">
+        <v>303</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -9158,6 +9232,9 @@
       <c r="D2" s="31"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -9168,7 +9245,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA42E1F6-175A-4BE2-8B97-2ABE974B15A6}">
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9176,13 +9255,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>315</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="A1" s="52" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="35"/>
@@ -9192,24 +9271,24 @@
       <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="52" t="s">
-        <v>316</v>
-      </c>
-      <c r="B3" s="52"/>
+      <c r="A3" s="49" t="s">
+        <v>312</v>
+      </c>
+      <c r="B3" s="49"/>
       <c r="C3" s="37" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="G3" s="38" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -9217,14 +9296,14 @@
         <v>0</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="D4" s="36"/>
       <c r="E4" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F4" s="39">
         <v>3</v>
@@ -9241,11 +9320,11 @@
         <v>65</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F5" s="39">
         <v>9</v>
@@ -9262,11 +9341,11 @@
         <v>66</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F6" s="39">
         <v>8</v>
@@ -9283,11 +9362,11 @@
         <v>67</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F7" s="39">
         <v>9</v>
@@ -9304,11 +9383,11 @@
         <v>68</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="D8" s="36"/>
       <c r="E8" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F8" s="39">
         <v>7</v>
@@ -9325,11 +9404,11 @@
         <v>69</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D9" s="36"/>
       <c r="E9" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F9" s="39">
         <v>6</v>
@@ -9346,11 +9425,11 @@
         <v>70</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D10" s="36"/>
       <c r="E10" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F10" s="39">
         <v>7</v>
@@ -9367,11 +9446,11 @@
         <v>71</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F11" s="39">
         <v>9</v>
@@ -9388,11 +9467,11 @@
         <v>72</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F12" s="39">
         <v>11</v>
@@ -9406,14 +9485,14 @@
         <v>9</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D13" s="36"/>
       <c r="E13" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F13" s="39">
         <v>8</v>
@@ -9427,14 +9506,14 @@
         <v>10</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F14" s="39">
         <v>10</v>
@@ -9448,14 +9527,14 @@
         <v>11</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D15" s="36"/>
       <c r="E15" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F15" s="39">
         <v>10</v>
@@ -9469,14 +9548,14 @@
         <v>12</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D16" s="36"/>
       <c r="E16" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F16" s="39">
         <v>8</v>
@@ -9490,14 +9569,14 @@
         <v>13</v>
       </c>
       <c r="B17" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="C17" s="36" t="s">
         <v>337</v>
-      </c>
-      <c r="C17" s="36" t="s">
-        <v>341</v>
       </c>
       <c r="D17" s="36"/>
       <c r="E17" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F17" s="39">
         <v>12</v>
@@ -9511,14 +9590,14 @@
         <v>14</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D18" s="36"/>
       <c r="E18" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F18" s="39">
         <v>8</v>
@@ -9532,14 +9611,14 @@
         <v>15</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D19" s="36"/>
       <c r="E19" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F19" s="39">
         <v>9</v>
@@ -9553,14 +9632,14 @@
         <v>16</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D20" s="36"/>
       <c r="E20" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F20" s="39">
         <v>8</v>
@@ -9574,14 +9653,14 @@
         <v>17</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="D21" s="36"/>
       <c r="E21" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F21" s="39">
         <v>8</v>
@@ -9595,14 +9674,14 @@
         <v>18</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D22" s="36"/>
       <c r="E22" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F22" s="39">
         <v>3</v>
@@ -9616,14 +9695,14 @@
         <v>19</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D23" s="36"/>
       <c r="E23" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F23" s="39">
         <v>9</v>
@@ -9637,14 +9716,14 @@
         <v>20</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D24" s="36"/>
       <c r="E24" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F24" s="39">
         <v>12</v>
@@ -9658,14 +9737,14 @@
         <v>21</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D25" s="36"/>
       <c r="E25" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F25" s="39">
         <v>12</v>
@@ -9679,14 +9758,14 @@
         <v>22</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D26" s="36"/>
       <c r="E26" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F26" s="39">
         <v>8</v>
@@ -9700,14 +9779,14 @@
         <v>23</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C27" s="36" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D27" s="36"/>
       <c r="E27" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F27" s="39">
         <v>11</v>
@@ -9728,14 +9807,14 @@
         <v>24</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C29" s="36" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D29" s="36"/>
       <c r="E29" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F29" s="39">
         <v>6</v>
@@ -9749,14 +9828,14 @@
         <v>25</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C30" s="36" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D30" s="36"/>
       <c r="E30" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F30" s="39">
         <v>9</v>
@@ -9770,14 +9849,14 @@
         <v>26</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D31" s="36"/>
       <c r="E31" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F31" s="39">
         <v>7</v>
@@ -9791,14 +9870,14 @@
         <v>27</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D32" s="36"/>
       <c r="E32" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F32" s="39">
         <v>8</v>
@@ -9812,14 +9891,14 @@
         <v>28</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C33" s="36" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D33" s="36"/>
       <c r="E33" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F33" s="39">
         <v>7</v>
@@ -9833,14 +9912,14 @@
         <v>29</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C34" s="36" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D34" s="36"/>
       <c r="E34" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F34" s="39">
         <v>7</v>
@@ -9854,14 +9933,14 @@
         <v>30</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C35" s="36" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D35" s="36"/>
       <c r="E35" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F35" s="39">
         <v>10</v>
@@ -9875,14 +9954,14 @@
         <v>31</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D36" s="36"/>
       <c r="E36" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F36" s="39">
         <v>3</v>
@@ -9896,14 +9975,14 @@
         <v>32</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D37" s="36"/>
       <c r="E37" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F37" s="39">
         <v>9</v>
@@ -9917,14 +9996,14 @@
         <v>33</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D38" s="36"/>
       <c r="E38" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F38" s="39">
         <v>11</v>
@@ -9938,14 +10017,14 @@
         <v>34</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D39" s="36"/>
       <c r="E39" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F39" s="39">
         <v>11</v>
@@ -9959,14 +10038,14 @@
         <v>35</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D40" s="36"/>
       <c r="E40" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F40" s="39">
         <v>9</v>
@@ -9980,14 +10059,14 @@
         <v>36</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D41" s="36"/>
       <c r="E41" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F41" s="39">
         <v>11</v>
@@ -10001,14 +10080,14 @@
         <v>37</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D42" s="36"/>
       <c r="E42" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F42" s="39">
         <v>9</v>
@@ -10022,14 +10101,14 @@
         <v>38</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D43" s="36"/>
       <c r="E43" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F43" s="39">
         <v>10</v>
@@ -10043,14 +10122,14 @@
         <v>39</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C44" s="36" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="D44" s="36"/>
       <c r="E44" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F44" s="39">
         <v>12</v>
@@ -10064,14 +10143,14 @@
         <v>40</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D45" s="36"/>
       <c r="E45" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F45" s="39">
         <v>6</v>
@@ -10085,14 +10164,14 @@
         <v>41</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="C46" s="36">
         <v>9</v>
       </c>
       <c r="D46" s="36"/>
       <c r="E46" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F46" s="39">
         <v>11</v>
@@ -10106,14 +10185,14 @@
         <v>42</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C47" s="36" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D47" s="36"/>
       <c r="E47" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F47" s="39">
         <v>10</v>
@@ -10127,14 +10206,14 @@
         <v>43</v>
       </c>
       <c r="B48" s="36" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C48" s="36">
         <v>3</v>
       </c>
       <c r="D48" s="36"/>
       <c r="E48" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F48" s="39">
         <v>7</v>
@@ -10148,14 +10227,14 @@
         <v>44</v>
       </c>
       <c r="B49" s="36" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C49" s="36" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D49" s="36"/>
       <c r="E49" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F49" s="39">
         <v>6</v>
@@ -10169,14 +10248,14 @@
         <v>45</v>
       </c>
       <c r="B50" s="36" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C50" s="36">
         <v>1</v>
       </c>
       <c r="D50" s="36"/>
       <c r="E50" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F50" s="39">
         <v>3</v>
@@ -10190,14 +10269,14 @@
         <v>46</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C51" s="36">
         <v>2</v>
       </c>
       <c r="D51" s="36"/>
       <c r="E51" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F51" s="39">
         <v>6</v>
@@ -10211,14 +10290,14 @@
         <v>47</v>
       </c>
       <c r="B52" s="36" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C52" s="36">
         <v>0</v>
       </c>
       <c r="D52" s="36"/>
       <c r="E52" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F52" s="39">
         <v>12</v>
@@ -10239,14 +10318,14 @@
         <v>48</v>
       </c>
       <c r="B54" s="36" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C54" s="36">
         <v>5</v>
       </c>
       <c r="D54" s="36"/>
       <c r="E54" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F54" s="39">
         <v>8</v>
@@ -10260,14 +10339,14 @@
         <v>49</v>
       </c>
       <c r="B55" s="36" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C55" s="36">
         <v>4</v>
       </c>
       <c r="D55" s="36"/>
       <c r="E55" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F55" s="39">
         <v>8</v>
@@ -10281,14 +10360,14 @@
         <v>50</v>
       </c>
       <c r="B56" s="36" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C56" s="36">
         <v>6</v>
       </c>
       <c r="D56" s="36"/>
       <c r="E56" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F56" s="39">
         <v>9</v>
@@ -10302,14 +10381,14 @@
         <v>51</v>
       </c>
       <c r="B57" s="36" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C57" s="36">
         <v>8</v>
       </c>
       <c r="D57" s="36"/>
       <c r="E57" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F57" s="39">
         <v>10</v>
@@ -10323,14 +10402,14 @@
         <v>52</v>
       </c>
       <c r="B58" s="36" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C58" s="36">
         <v>7</v>
       </c>
       <c r="D58" s="36"/>
       <c r="E58" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F58" s="39">
         <v>9</v>
@@ -10344,14 +10423,14 @@
         <v>53</v>
       </c>
       <c r="B59" s="36" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C59" s="36" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D59" s="36"/>
       <c r="E59" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F59" s="39">
         <v>10</v>
@@ -10365,14 +10444,14 @@
         <v>54</v>
       </c>
       <c r="B60" s="36" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C60" s="36" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D60" s="36"/>
       <c r="E60" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F60" s="39">
         <v>8</v>
@@ -10386,14 +10465,14 @@
         <v>55</v>
       </c>
       <c r="B61" s="36" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C61" s="36" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="D61" s="36"/>
       <c r="E61" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F61" s="39">
         <v>7</v>
@@ -10407,14 +10486,14 @@
         <v>56</v>
       </c>
       <c r="B62" s="36" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C62" s="36" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D62" s="36"/>
       <c r="E62" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F62" s="39">
         <v>8</v>
@@ -10428,16 +10507,16 @@
         <v>57</v>
       </c>
       <c r="B63" s="36" t="s">
+        <v>411</v>
+      </c>
+      <c r="C63" s="36" t="s">
+        <v>414</v>
+      </c>
+      <c r="D63" s="36" t="s">
         <v>415</v>
       </c>
-      <c r="C63" s="36" t="s">
-        <v>418</v>
-      </c>
-      <c r="D63" s="36" t="s">
-        <v>419</v>
-      </c>
       <c r="E63" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F63" s="39">
         <v>9</v>
@@ -10451,14 +10530,14 @@
         <v>58</v>
       </c>
       <c r="B64" s="36" t="s">
+        <v>413</v>
+      </c>
+      <c r="C64" s="36" t="s">
         <v>417</v>
-      </c>
-      <c r="C64" s="36" t="s">
-        <v>421</v>
       </c>
       <c r="D64" s="36"/>
       <c r="E64" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F64" s="39">
         <v>10</v>
@@ -10472,16 +10551,16 @@
         <v>59</v>
       </c>
       <c r="B65" s="36" t="s">
+        <v>416</v>
+      </c>
+      <c r="C65" s="36" t="s">
+        <v>419</v>
+      </c>
+      <c r="D65" s="36" t="s">
         <v>420</v>
       </c>
-      <c r="C65" s="36" t="s">
-        <v>423</v>
-      </c>
-      <c r="D65" s="36" t="s">
-        <v>424</v>
-      </c>
       <c r="E65" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F65" s="39">
         <v>3</v>
@@ -10495,14 +10574,14 @@
         <v>60</v>
       </c>
       <c r="B66" s="36" t="s">
+        <v>418</v>
+      </c>
+      <c r="C66" s="36" t="s">
         <v>422</v>
-      </c>
-      <c r="C66" s="36" t="s">
-        <v>426</v>
       </c>
       <c r="D66" s="36"/>
       <c r="E66" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F66" s="39">
         <v>6</v>
@@ -10516,14 +10595,14 @@
         <v>61</v>
       </c>
       <c r="B67" s="36" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C67" s="36" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="D67" s="36"/>
       <c r="E67" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F67" s="39">
         <v>3</v>
@@ -10537,14 +10616,14 @@
         <v>62</v>
       </c>
       <c r="B68" s="36" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C68" s="36" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D68" s="36"/>
       <c r="E68" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F68" s="39">
         <v>9</v>
@@ -10558,14 +10637,14 @@
         <v>63</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C69" s="36" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="D69" s="36"/>
       <c r="E69" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F69" s="39">
         <v>10</v>
@@ -10579,14 +10658,14 @@
         <v>64</v>
       </c>
       <c r="B70" s="36" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C70" s="36" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="D70" s="36"/>
       <c r="E70" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F70" s="39">
         <v>10</v>
@@ -10600,16 +10679,16 @@
         <v>65</v>
       </c>
       <c r="B71" s="36" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="C71" s="36" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D71" s="36" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="E71" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F71" s="39">
         <v>12</v>
@@ -10623,16 +10702,16 @@
         <v>66</v>
       </c>
       <c r="B72" s="36" t="s">
+        <v>431</v>
+      </c>
+      <c r="C72" s="36" t="s">
         <v>435</v>
       </c>
-      <c r="C72" s="36" t="s">
-        <v>439</v>
-      </c>
       <c r="D72" s="36" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="E72" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F72" s="39">
         <v>10</v>
@@ -10647,16 +10726,16 @@
         <v>67</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C73" s="36" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="D73" s="36" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="E73" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F73" s="39">
         <v>3</v>
@@ -10670,16 +10749,16 @@
         <v>68</v>
       </c>
       <c r="B74" s="36" t="s">
+        <v>438</v>
+      </c>
+      <c r="C74" s="36" t="s">
         <v>442</v>
       </c>
-      <c r="C74" s="36" t="s">
-        <v>446</v>
-      </c>
       <c r="D74" s="36" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="E74" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F74" s="39">
         <v>12</v>
@@ -10693,16 +10772,16 @@
         <v>69</v>
       </c>
       <c r="B75" s="36" t="s">
+        <v>441</v>
+      </c>
+      <c r="C75" s="36" t="s">
         <v>445</v>
       </c>
-      <c r="C75" s="36" t="s">
-        <v>449</v>
-      </c>
       <c r="D75" s="36" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E75" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F75" s="39">
         <v>12</v>
@@ -10716,16 +10795,16 @@
         <v>70</v>
       </c>
       <c r="B76" s="36" t="s">
+        <v>444</v>
+      </c>
+      <c r="C76" s="36" t="s">
         <v>448</v>
       </c>
-      <c r="C76" s="36" t="s">
-        <v>452</v>
-      </c>
       <c r="D76" s="36" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="E76" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F76" s="39">
         <v>12</v>
@@ -10739,16 +10818,16 @@
         <v>71</v>
       </c>
       <c r="B77" s="36" t="s">
+        <v>447</v>
+      </c>
+      <c r="C77" s="36" t="s">
         <v>451</v>
       </c>
-      <c r="C77" s="36" t="s">
-        <v>455</v>
-      </c>
       <c r="D77" s="36" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="E77" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F77" s="39">
         <v>12</v>
@@ -10771,14 +10850,14 @@
         <v>72</v>
       </c>
       <c r="B79" s="36" t="s">
+        <v>450</v>
+      </c>
+      <c r="C79" s="36" t="s">
         <v>454</v>
-      </c>
-      <c r="C79" s="36" t="s">
-        <v>458</v>
       </c>
       <c r="D79" s="36"/>
       <c r="E79" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F79" s="39">
         <v>3</v>
@@ -10792,14 +10871,14 @@
         <v>73</v>
       </c>
       <c r="B80" s="36" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C80" s="36" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D80" s="36"/>
       <c r="E80" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F80" s="39">
         <v>12</v>
@@ -10813,14 +10892,14 @@
         <v>74</v>
       </c>
       <c r="B81" s="36" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C81" s="36" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="D81" s="36"/>
       <c r="E81" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F81" s="39">
         <v>12</v>
@@ -10834,14 +10913,14 @@
         <v>75</v>
       </c>
       <c r="B82" s="36" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C82" s="36" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D82" s="36"/>
       <c r="E82" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F82" s="39">
         <v>12</v>
@@ -10855,14 +10934,14 @@
         <v>76</v>
       </c>
       <c r="B83" s="36" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C83" s="36" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="D83" s="36"/>
       <c r="E83" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F83" s="39">
         <v>10</v>
@@ -10876,14 +10955,14 @@
         <v>77</v>
       </c>
       <c r="B84" s="36" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C84" s="36" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="D84" s="36"/>
       <c r="E84" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F84" s="39">
         <v>12</v>
@@ -10897,14 +10976,14 @@
         <v>78</v>
       </c>
       <c r="B85" s="36" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C85" s="36" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="D85" s="36"/>
       <c r="E85" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F85" s="39">
         <v>12</v>
@@ -10918,14 +10997,14 @@
         <v>79</v>
       </c>
       <c r="B86" s="36" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C86" s="36" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="D86" s="36"/>
       <c r="E86" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F86" s="39">
         <v>12</v>
@@ -10939,14 +11018,14 @@
         <v>80</v>
       </c>
       <c r="B87" s="36" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C87" s="36" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="D87" s="36"/>
       <c r="E87" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F87" s="39">
         <v>6</v>
@@ -10960,14 +11039,14 @@
         <v>81</v>
       </c>
       <c r="B88" s="36" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C88" s="36" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="D88" s="36"/>
       <c r="E88" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F88" s="39">
         <v>12</v>
@@ -10981,14 +11060,14 @@
         <v>82</v>
       </c>
       <c r="B89" s="36" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C89" s="36" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="D89" s="36"/>
       <c r="E89" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F89" s="39">
         <v>8</v>
@@ -11002,14 +11081,14 @@
         <v>83</v>
       </c>
       <c r="B90" s="36" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C90" s="36" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D90" s="36"/>
       <c r="E90" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F90" s="39">
         <v>3</v>
@@ -11023,14 +11102,14 @@
         <v>84</v>
       </c>
       <c r="B91" s="36" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C91" s="36" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D91" s="36"/>
       <c r="E91" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F91" s="39">
         <v>6</v>
@@ -11044,14 +11123,14 @@
         <v>85</v>
       </c>
       <c r="B92" s="36" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C92" s="36" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="D92" s="36"/>
       <c r="E92" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F92" s="39">
         <v>9</v>
@@ -11065,14 +11144,14 @@
         <v>86</v>
       </c>
       <c r="B93" s="36" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C93" s="36" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D93" s="36"/>
       <c r="E93" s="36" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F93" s="39">
         <v>11</v>
@@ -11086,14 +11165,14 @@
         <v>87</v>
       </c>
       <c r="B94" s="36" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C94" s="36" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="D94" s="36"/>
       <c r="E94" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F94" s="39">
         <v>9</v>
@@ -11107,14 +11186,14 @@
         <v>88</v>
       </c>
       <c r="B95" s="36" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C95" s="36" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="D95" s="36"/>
       <c r="E95" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F95" s="39">
         <v>8</v>
@@ -11128,14 +11207,14 @@
         <v>89</v>
       </c>
       <c r="B96" s="36" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C96" s="36" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="D96" s="36"/>
       <c r="E96" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F96" s="39">
         <v>8</v>
@@ -11149,14 +11228,14 @@
         <v>90</v>
       </c>
       <c r="B97" s="36" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C97" s="36" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="D97" s="36"/>
       <c r="E97" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F97" s="39">
         <v>9</v>
@@ -11170,14 +11249,14 @@
         <v>91</v>
       </c>
       <c r="B98" s="36" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C98" s="36" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="D98" s="36"/>
       <c r="E98" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F98" s="39">
         <v>3</v>
@@ -11191,14 +11270,14 @@
         <v>92</v>
       </c>
       <c r="B99" s="36" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C99" s="36" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="D99" s="36"/>
       <c r="E99" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F99" s="39">
         <v>10</v>
@@ -11212,14 +11291,14 @@
         <v>93</v>
       </c>
       <c r="B100" s="36" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C100" s="36" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="D100" s="36"/>
       <c r="E100" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F100" s="39">
         <v>8</v>
@@ -11233,14 +11312,14 @@
         <v>94</v>
       </c>
       <c r="B101" s="36" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C101" s="36" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D101" s="36"/>
       <c r="E101" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F101" s="39">
         <v>11</v>
@@ -11254,14 +11333,14 @@
         <v>95</v>
       </c>
       <c r="B102" s="36" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C102" s="36" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="D102" s="36"/>
       <c r="E102" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F102" s="39">
         <v>7</v>
@@ -11295,8 +11374,9 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:H102">
     <sortCondition ref="A4:A102"/>
   </sortState>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11307,7 +11387,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A09231-9234-4663-AC2B-A7E153BD7254}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11316,35 +11398,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>511</v>
-      </c>
-      <c r="B1" s="43"/>
+      <c r="A1" s="52" t="s">
+        <v>580</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="36"/>
     </row>
     <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="44" t="s">
-        <v>510</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>319</v>
+      <c r="A3" s="40" t="s">
+        <v>506</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>315</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C4" s="39">
         <v>1</v>
@@ -11355,10 +11439,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C5" s="39">
         <v>1</v>
@@ -11369,10 +11453,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C6" s="39">
         <v>2</v>
@@ -11383,10 +11467,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C7" s="39">
         <v>2</v>
@@ -11397,10 +11481,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C8" s="39">
         <v>2</v>
@@ -11411,10 +11495,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C9" s="39">
         <v>2</v>
@@ -11425,10 +11509,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C10" s="39">
         <v>2</v>
@@ -11439,10 +11523,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C11" s="39">
         <v>2</v>
@@ -11453,10 +11537,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C12" s="39">
         <v>2</v>
@@ -11467,10 +11551,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C13" s="39">
         <v>2</v>
@@ -11481,10 +11565,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C14" s="39">
         <v>2</v>
@@ -11495,10 +11579,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C15" s="39">
         <v>2</v>
@@ -11509,10 +11593,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C16" s="39">
         <v>3</v>
@@ -11523,10 +11607,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C17" s="39">
         <v>3</v>
@@ -11537,10 +11621,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C18" s="39">
         <v>4</v>
@@ -11551,10 +11635,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C19" s="39">
         <v>4</v>
@@ -11565,10 +11649,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="36" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C20" s="39">
         <v>4</v>
@@ -11579,10 +11663,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C21" s="39">
         <v>4</v>
@@ -11593,10 +11677,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C22" s="39">
         <v>4</v>
@@ -11607,10 +11691,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C23" s="39">
         <v>4</v>
@@ -11621,10 +11705,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="36" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C24" s="39">
         <v>4</v>
@@ -11635,10 +11719,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C25" s="39">
         <v>5</v>
@@ -11649,10 +11733,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="36" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C26" s="39">
         <v>6</v>
@@ -11663,10 +11747,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="36" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C27" s="39">
         <v>6</v>
@@ -11677,10 +11761,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="36" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C28" s="39">
         <v>7</v>
@@ -11691,10 +11775,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C29" s="39">
         <v>7</v>
@@ -11705,10 +11789,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="36" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C30" s="39">
         <v>7</v>
@@ -11719,10 +11803,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C31" s="39">
         <v>8</v>
@@ -11733,10 +11817,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C32" s="39">
         <v>8</v>
@@ -11747,10 +11831,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C33" s="39">
         <v>8</v>
@@ -11761,10 +11845,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="36" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C34" s="39">
         <v>9</v>
@@ -11775,10 +11859,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C35" s="39">
         <v>9</v>
@@ -11788,11 +11872,11 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="53" t="s">
-        <v>541</v>
+      <c r="A36" s="41" t="s">
+        <v>536</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C36" s="39">
         <v>9</v>
@@ -11803,10 +11887,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="36" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C37" s="39">
         <v>9</v>
@@ -11816,11 +11900,11 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="53" t="s">
-        <v>515</v>
+      <c r="A38" s="41" t="s">
+        <v>510</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C38" s="39">
         <v>10</v>
@@ -11831,10 +11915,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="36" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C39" s="39">
         <v>11</v>
@@ -11845,10 +11929,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="36" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C40" s="39">
         <v>11</v>
@@ -11859,10 +11943,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="36" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C41" s="39">
         <v>11</v>
@@ -11873,10 +11957,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="36" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C42" s="39">
         <v>13</v>
@@ -11887,10 +11971,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="36" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C43" s="39">
         <v>13</v>
@@ -11901,10 +11985,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="36" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C44" s="39">
         <v>13</v>
@@ -11915,10 +11999,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="36" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C45" s="39">
         <v>13</v>
@@ -11929,10 +12013,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="36" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C46" s="39">
         <v>13</v>
@@ -11943,10 +12027,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="36" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C47" s="39">
         <v>13</v>
@@ -11957,10 +12041,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="36" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="B48" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C48" s="39">
         <v>13</v>
@@ -11971,10 +12055,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="36" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="B49" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C49" s="39">
         <v>13</v>
@@ -11985,10 +12069,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="36" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="B50" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C50" s="39">
         <v>14</v>
@@ -11999,10 +12083,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="36" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C51" s="39">
         <v>14</v>
@@ -12013,10 +12097,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="36" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="B52" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C52" s="39">
         <v>14</v>
@@ -12027,10 +12111,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="36" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="B53" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C53" s="39">
         <v>14</v>
@@ -12041,10 +12125,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="36" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="B54" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C54" s="39">
         <v>14</v>
@@ -12055,10 +12139,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="36" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="B55" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C55" s="39">
         <v>14</v>
@@ -12069,10 +12153,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="36" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="B56" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C56" s="39">
         <v>14</v>
@@ -12083,10 +12167,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="36" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="B57" s="36" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C57" s="39">
         <v>14</v>
@@ -12097,10 +12181,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="36" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="B58" s="36" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C58" s="39">
         <v>14</v>
@@ -12301,6 +12385,9 @@
       <c r="B105" s="36"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -12320,12 +12407,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>302</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="A1" s="50" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -12334,6 +12421,9 @@
       <c r="D2" s="31"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -12347,7 +12437,9 @@
   </sheetPr>
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12358,31 +12450,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>268</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="A1" s="50" t="s">
+        <v>265</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="45" t="s">
-        <v>269</v>
-      </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
+      <c r="D2" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -12432,57 +12524,57 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="43" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>283</v>
-      </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="32" t="s">
         <v>63</v>
       </c>
@@ -12537,7 +12629,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>65</v>
@@ -12580,7 +12672,7 @@
         <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>66</v>
@@ -12595,7 +12687,7 @@
         <v>84</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
@@ -12629,7 +12721,7 @@
         <v>73</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>67</v>
@@ -12640,7 +12732,7 @@
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="33" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -12652,11 +12744,11 @@
         <v>128</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="22" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="24" t="s">
@@ -12668,7 +12760,7 @@
         <v>74</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>68</v>
@@ -12688,7 +12780,7 @@
         <v>111</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="K9" s="22" t="s">
         <v>121</v>
@@ -12703,13 +12795,13 @@
         <v>139</v>
       </c>
       <c r="O9" s="22" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="P9" s="33" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -12717,7 +12809,7 @@
         <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>69</v>
@@ -12730,7 +12822,7 @@
         <v>86</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="22" t="s">
@@ -12752,10 +12844,10 @@
         <v>140</v>
       </c>
       <c r="O10" s="22" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="P10" s="33" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="Q10" s="15"/>
     </row>
@@ -12764,7 +12856,7 @@
         <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>70</v>
@@ -12774,10 +12866,10 @@
         <v>80</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="G11" s="33" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
@@ -12786,7 +12878,7 @@
         <v>123</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="M11" s="22" t="s">
         <v>136</v>
@@ -12799,7 +12891,7 @@
         <v>150</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -12807,7 +12899,7 @@
         <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>71</v>
@@ -12820,7 +12912,7 @@
         <v>87</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="22" t="s">
@@ -12830,10 +12922,10 @@
         <v>117</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="M12" s="22" t="s">
         <v>137</v>
@@ -12842,13 +12934,13 @@
         <v>141</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="P12" s="33" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="Q12" s="24" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -12856,7 +12948,7 @@
         <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>72</v>
@@ -12867,7 +12959,7 @@
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="23" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
@@ -12881,37 +12973,38 @@
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="23" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="P13" s="23" t="s">
         <v>152</v>
       </c>
       <c r="Q13" s="34" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="48" t="s">
-        <v>299</v>
-      </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
+      <c r="B16" s="45" t="s">
+        <v>296</v>
+      </c>
+      <c r="C16" s="46"/>
+      <c r="D16" s="47"/>
     </row>
     <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="51" t="s">
-        <v>300</v>
-      </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
+      <c r="B18" s="48" t="s">
+        <v>297</v>
+      </c>
+      <c r="C18" s="46"/>
+      <c r="D18" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="96" fitToWidth="0" orientation="landscape" r:id="rId1"/>
@@ -12932,12 +13025,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>303</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="A1" s="50" t="s">
+        <v>300</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -12946,6 +13039,9 @@
       <c r="D2" s="31"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -12959,7 +13055,9 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12970,31 +13068,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>266</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="A1" s="50" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -13044,7 +13142,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="43" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -13094,7 +13192,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -13170,18 +13268,18 @@
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
       <c r="O6" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q6" s="27"/>
     </row>
@@ -13203,30 +13301,30 @@
         <v>102</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="O7" s="14"/>
       <c r="P7" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q7" s="24" t="s">
         <v>154</v>
@@ -13250,19 +13348,19 @@
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M8" s="26"/>
       <c r="N8" s="14"/>
       <c r="O8" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="24" t="s">
-        <v>155</v>
+        <v>582</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -13281,33 +13379,33 @@
         <v>93</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>104</v>
+        <v>581</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N9" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O9" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -13328,19 +13426,19 @@
       <c r="I10" s="26"/>
       <c r="J10" s="26"/>
       <c r="K10" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N10" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O10" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="15"/>
@@ -13367,23 +13465,23 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
       <c r="K11" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>202</v>
+        <v>583</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -13404,29 +13502,29 @@
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="24" t="s">
-        <v>156</v>
+        <v>584</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -13445,31 +13543,32 @@
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="23" t="s">
-        <v>579</v>
+        <v>585</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P13" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q13" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="96" fitToWidth="0" orientation="landscape" r:id="rId1"/>
@@ -13490,12 +13589,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>304</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="A1" s="50" t="s">
+        <v>301</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
@@ -13504,6 +13603,9 @@
       <c r="D2" s="31"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -13517,7 +13619,9 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13528,29 +13632,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="41"/>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -13600,7 +13704,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="43" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -13650,7 +13754,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -13721,15 +13825,15 @@
         <v>96</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -13737,10 +13841,10 @@
         <v>142</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -13761,30 +13865,30 @@
         <v>98</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>158</v>
+        <v>310</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="O7" s="14"/>
       <c r="P7" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q7" s="24" t="s">
         <v>154</v>
@@ -13808,17 +13912,17 @@
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="22" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="22" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="24" t="s">
@@ -13847,29 +13951,29 @@
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="22" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="M9" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="N9" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="N9" s="22" t="s">
-        <v>228</v>
-      </c>
       <c r="O9" s="22" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -13890,13 +13994,13 @@
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="22" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="L10" s="22" t="s">
         <v>130</v>
@@ -13905,7 +14009,7 @@
         <v>135</v>
       </c>
       <c r="N10" s="22" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O10" s="22" t="s">
         <v>144</v>
@@ -13928,7 +14032,7 @@
         <v>91</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -13938,7 +14042,7 @@
         <v>123</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M11" s="22" t="s">
         <v>136</v>
@@ -13948,10 +14052,10 @@
         <v>145</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>236</v>
+        <v>586</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -13972,25 +14076,25 @@
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="22" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="24" t="s">
@@ -14013,31 +14117,32 @@
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="23" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="23" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="P13" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q13" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="96" fitToWidth="0" orientation="landscape" r:id="rId1"/>
@@ -14058,11 +14163,11 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>305</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
+      <c r="A1" s="50" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
       <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14072,6 +14177,9 @@
       <c r="D2" s="31"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -14085,7 +14193,9 @@
   </sheetPr>
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14096,31 +14206,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>267</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="A1" s="50" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
@@ -14170,7 +14280,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="43" t="s">
         <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -14220,7 +14330,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
+      <c r="A5" s="44"/>
       <c r="B5" s="4" t="s">
         <v>63</v>
       </c>
@@ -14291,15 +14401,15 @@
         <v>96</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="K6" s="21" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -14307,10 +14417,10 @@
         <v>142</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q6" s="25" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -14328,33 +14438,33 @@
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="22" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="J7" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="J7" s="22" t="s">
-        <v>245</v>
-      </c>
       <c r="K7" s="22" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="O7" s="14"/>
       <c r="P7" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q7" s="24" t="s">
         <v>154</v>
@@ -14378,17 +14488,17 @@
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="22" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="22" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="24" t="s">
@@ -14407,39 +14517,39 @@
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="22" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G9" s="22" t="s">
         <v>104</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="J9" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="J9" s="22" t="s">
-        <v>246</v>
-      </c>
       <c r="K9" s="22" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="M9" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="N9" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="N9" s="22" t="s">
-        <v>263</v>
-      </c>
       <c r="O9" s="22" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -14460,13 +14570,13 @@
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="22" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="L10" s="22" t="s">
         <v>130</v>
@@ -14475,7 +14585,7 @@
         <v>135</v>
       </c>
       <c r="N10" s="22" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O10" s="22" t="s">
         <v>144</v>
@@ -14498,7 +14608,7 @@
         <v>91</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -14508,7 +14618,7 @@
         <v>123</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M11" s="22" t="s">
         <v>136</v>
@@ -14518,10 +14628,10 @@
         <v>145</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>236</v>
+        <v>586</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -14536,33 +14646,33 @@
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="22" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="J12" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="J12" s="22" t="s">
-        <v>247</v>
-      </c>
       <c r="K12" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="L12" s="22" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="M12" s="22" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="N12" s="22" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="24" t="s">
@@ -14585,31 +14695,32 @@
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="23" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
       <c r="K13" s="23" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="23" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="P13" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q13" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D2:Q2"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="96" fitToWidth="0" orientation="landscape" r:id="rId1"/>

</xml_diff>